<commit_message>
feat - atualizado template - planilha agora utiliza lib openpyxl
</commit_message>
<xml_diff>
--- a/template.xlsx
+++ b/template.xlsx
@@ -8,14 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luan\Documents\Projetos\Entercap\ENTERCAP-Resumo-tributario\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AC4E923-F019-43DF-BBC7-0ECD8F757021}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11250B43-2859-4F09-8AB4-F00C4E195E27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Apresentação" sheetId="4" r:id="rId1"/>
     <sheet name="Planejamento Tributário" sheetId="2" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="CNPJ">Apresentação!$C$7</definedName>
+    <definedName name="EMPRESA">Apresentação!$B$7</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -35,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="75">
   <si>
     <t>1410 - INSS</t>
   </si>
@@ -131,9 +135,6 @@
   </si>
   <si>
     <t>Cofins</t>
-  </si>
-  <si>
-    <t>CNPJ: 16.684.262/0001-52</t>
   </si>
   <si>
     <t>Planejamento Tributário: Oportunidades Lucro Presumido x Lucro Real</t>
@@ -540,7 +541,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="98">
+  <cellXfs count="99">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
@@ -667,10 +668,13 @@
     <xf numFmtId="43" fontId="6" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="43" fontId="3" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Moeda" xfId="3" builtinId="4"/>
@@ -1685,8 +1689,8 @@
   </sheetPr>
   <dimension ref="A7:S71"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1715,25 +1719,26 @@
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="52"/>
       <c r="B7" s="49" t="s">
+        <v>73</v>
+      </c>
+      <c r="C7" s="98" t="s">
         <v>74</v>
       </c>
-      <c r="D7" s="52" t="s">
-        <v>75</v>
-      </c>
+      <c r="D7" s="52"/>
       <c r="H7" s="2"/>
     </row>
     <row r="10" spans="1:16" ht="21" x14ac:dyDescent="0.35">
       <c r="B10" s="42" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C10" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="11" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B12" s="13" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C12" s="46"/>
       <c r="D12" s="46"/>
@@ -1743,7 +1748,7 @@
       <c r="H12" s="15"/>
       <c r="N12"/>
       <c r="O12" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="P12" s="80">
         <f>C43</f>
@@ -1759,11 +1764,11 @@
         <v>27</v>
       </c>
       <c r="H13" s="18" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="N13"/>
       <c r="O13" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="P13" s="80">
         <f>C44</f>
@@ -1772,7 +1777,7 @@
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B14" s="10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F14" s="58">
         <v>100000</v>
@@ -1820,7 +1825,7 @@
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B16" s="10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F16" s="58">
         <v>2000</v>
@@ -1834,7 +1839,7 @@
       </c>
       <c r="N16"/>
       <c r="O16" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="P16" s="1">
         <f>F15</f>
@@ -1848,7 +1853,7 @@
       <c r="H17" s="12"/>
       <c r="N17"/>
       <c r="O17" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="P17" s="1">
         <f>F30</f>
@@ -1857,7 +1862,7 @@
     </row>
     <row r="18" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B18" s="10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F18" s="58">
         <v>3000</v>
@@ -1871,7 +1876,7 @@
       </c>
       <c r="N18"/>
       <c r="O18" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="P18" s="1">
         <f>F14</f>
@@ -1880,7 +1885,7 @@
     </row>
     <row r="19" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B19" s="10" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F19" s="58">
         <f>0.08*F16</f>
@@ -1896,15 +1901,15 @@
       <c r="J19" s="3"/>
       <c r="N19" s="82"/>
       <c r="O19" s="83" t="s">
+        <v>58</v>
+      </c>
+      <c r="P19" s="84" t="s">
         <v>59</v>
-      </c>
-      <c r="P19" s="84" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="20" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B20" s="10" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F20" s="58">
         <v>4000</v>
@@ -1920,7 +1925,7 @@
       <c r="L20" s="58"/>
       <c r="M20" s="74"/>
       <c r="N20" s="85" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="O20" s="76">
         <f>(P16-O24)</f>
@@ -1930,7 +1935,7 @@
     </row>
     <row r="21" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B21" s="10" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F21" s="58">
         <v>3000</v>
@@ -1946,7 +1951,7 @@
       <c r="L21" s="58"/>
       <c r="M21" s="74"/>
       <c r="N21" s="85" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="O21" s="1">
         <f>P17</f>
@@ -1956,7 +1961,7 @@
     </row>
     <row r="22" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B22" s="47" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F22" s="58">
         <v>5000</v>
@@ -1972,7 +1977,7 @@
       <c r="L22" s="79"/>
       <c r="M22" s="74"/>
       <c r="N22" s="85" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="P22" s="90">
         <f>(P18-P24)</f>
@@ -1988,7 +1993,7 @@
     </row>
     <row r="23" spans="2:19" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B23" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F23" s="58">
         <v>6000</v>
@@ -2004,7 +2009,7 @@
       <c r="L23" s="79"/>
       <c r="M23" s="74"/>
       <c r="N23" s="91" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="O23" s="92">
         <f>SUM(O20:O22)</f>
@@ -2024,7 +2029,7 @@
     </row>
     <row r="24" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B24" s="10" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F24" s="58">
         <v>7000</v>
@@ -2041,7 +2046,7 @@
       <c r="L24" s="79"/>
       <c r="M24" s="74"/>
       <c r="N24" s="87" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="O24" s="88">
         <f>P16*P12</f>
@@ -2054,7 +2059,7 @@
     </row>
     <row r="25" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B25" s="10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F25" s="58">
         <v>8000</v>
@@ -2071,13 +2076,13 @@
       <c r="L25" s="79"/>
       <c r="M25" s="74"/>
       <c r="N25" s="75">
-        <f t="shared" ref="N23:N25" si="1">+K25*30*L25</f>
+        <f t="shared" ref="N25" si="1">+K25*30*L25</f>
         <v>0</v>
       </c>
     </row>
     <row r="26" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B26" s="19" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C26" s="45"/>
       <c r="D26" s="45"/>
@@ -2127,7 +2132,7 @@
     </row>
     <row r="29" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B29" s="19" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C29" s="45"/>
       <c r="D29" s="45"/>
@@ -2138,14 +2143,14 @@
     </row>
     <row r="30" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B30" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C30" s="59">
         <f>F30/16</f>
         <v>2500</v>
       </c>
       <c r="D30" s="60" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F30" s="58">
         <f>H30*F14</f>
@@ -2161,14 +2166,14 @@
     </row>
     <row r="31" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B31" s="10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C31" s="59">
         <f>F31/16</f>
         <v>1249.9999999999984</v>
       </c>
       <c r="D31" s="60" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F31" s="58">
         <f>G31*F14</f>
@@ -2182,7 +2187,7 @@
     </row>
     <row r="32" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B32" s="27" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C32" s="28"/>
       <c r="D32" s="28"/>
@@ -2219,7 +2224,7 @@
     </row>
     <row r="36" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B36" s="10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F36" s="58">
         <f>F14*H36</f>
@@ -2233,12 +2238,12 @@
         <v>1.6179207781519361E-2</v>
       </c>
       <c r="L36" s="57"/>
-      <c r="O36" s="97"/>
-      <c r="P36" s="97"/>
+      <c r="O36" s="96"/>
+      <c r="P36" s="96"/>
     </row>
     <row r="37" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B37" s="10" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F37" s="58">
         <f>S23</f>
@@ -2252,12 +2257,12 @@
         <v>7.5999999999999998E-2</v>
       </c>
       <c r="L37" s="3"/>
-      <c r="O37" s="97"/>
-      <c r="P37" s="97"/>
+      <c r="O37" s="96"/>
+      <c r="P37" s="96"/>
     </row>
     <row r="38" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B38" s="10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F38" s="58">
         <f>S22</f>
@@ -2270,12 +2275,12 @@
       <c r="H38" s="61">
         <v>1.6500000000000001E-2</v>
       </c>
-      <c r="O38" s="97"/>
-      <c r="P38" s="97"/>
+      <c r="O38" s="96"/>
+      <c r="P38" s="96"/>
     </row>
     <row r="39" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B39" s="10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F39" s="58">
         <f>IF(F31&gt;0,F31*H39,0)</f>
@@ -2288,12 +2293,12 @@
       <c r="H39" s="61">
         <v>0.15</v>
       </c>
-      <c r="O39" s="97"/>
-      <c r="P39" s="97"/>
+      <c r="O39" s="96"/>
+      <c r="P39" s="96"/>
     </row>
     <row r="40" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B40" s="10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F40" s="58">
         <f>IF(F31&gt;0,F31*H40,0)</f>
@@ -2306,8 +2311,8 @@
       <c r="H40" s="61">
         <v>0.09</v>
       </c>
-      <c r="O40" s="97"/>
-      <c r="P40" s="97"/>
+      <c r="O40" s="96"/>
+      <c r="P40" s="96"/>
     </row>
     <row r="41" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B41" s="10" t="s">
@@ -2335,7 +2340,7 @@
     </row>
     <row r="43" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B43" s="10" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C43" s="80">
         <v>0.12</v>
@@ -2346,7 +2351,7 @@
     </row>
     <row r="44" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B44" s="10" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C44" s="80">
         <v>0.12</v>
@@ -2395,7 +2400,7 @@
     </row>
     <row r="49" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B49" s="68" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C49" s="69"/>
       <c r="D49" s="69"/>
@@ -2424,7 +2429,7 @@
     </row>
     <row r="52" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B52" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G52" s="1" t="s">
         <v>30</v>
@@ -2433,7 +2438,7 @@
     </row>
     <row r="53" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B53" s="10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G53" s="1" t="s">
         <v>30</v>
@@ -2479,10 +2484,10 @@
       <c r="D60" s="4"/>
     </row>
     <row r="65" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B65" s="96" t="s">
+      <c r="B65" s="97" t="s">
         <v>16</v>
       </c>
-      <c r="C65" s="96"/>
+      <c r="C65" s="97"/>
     </row>
     <row r="66" spans="2:3" ht="11.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B66" t="s">
@@ -2532,8 +2537,8 @@
   </sheetPr>
   <dimension ref="B7:H59"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L29" sqref="L29:N37"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2545,16 +2550,18 @@
   </cols>
   <sheetData>
     <row r="7" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B7" s="49" t="s">
-        <v>74</v>
-      </c>
-      <c r="D7" t="s">
-        <v>32</v>
+      <c r="B7" s="49" t="str">
+        <f>EMPRESA</f>
+        <v>Empresa: NOME EMPRESA LTDA</v>
+      </c>
+      <c r="D7" s="98" t="str">
+        <f>CNPJ</f>
+        <v>CNPJ: 00.111.222/0001-03</v>
       </c>
     </row>
     <row r="10" spans="2:8" ht="21" x14ac:dyDescent="0.35">
       <c r="B10" s="42" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="11" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -2849,7 +2856,7 @@
     </row>
     <row r="38" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B38" s="32" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C38" s="44"/>
       <c r="D38" s="44"/>
@@ -2948,10 +2955,10 @@
       </c>
     </row>
     <row r="53" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B53" s="96" t="s">
+      <c r="B53" s="97" t="s">
         <v>16</v>
       </c>
-      <c r="C53" s="96"/>
+      <c r="C53" s="97"/>
     </row>
     <row r="54" spans="2:3" ht="11.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B54" t="s">

</xml_diff>

<commit_message>
feat - receitas com e sem st agora ficam abaixo de faturamento - icms fica acima de margens de lucro e custo - nova funcao para adicionar valor na apresentação acima de qualquer linha com uma descricao X
</commit_message>
<xml_diff>
--- a/template.xlsx
+++ b/template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luan\Documents\Projetos\Entercap\ENTERCAP-Resumo-tributario\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BF8577A-1810-49CD-8B0B-B0DF158F3E47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11D44A26-CC3E-4EC2-9E73-0DACF2DF7001}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="56">
   <si>
     <t>COMPRAS</t>
   </si>
@@ -198,6 +198,15 @@
   </si>
   <si>
     <t>DESCRIÇÃO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Receita sem ST </t>
+  </si>
+  <si>
+    <t>Receita com ST</t>
+  </si>
+  <si>
+    <t>b</t>
   </si>
 </sst>
 </file>
@@ -627,13 +636,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>222250</xdr:colOff>
-      <xdr:row>57</xdr:row>
+      <xdr:row>59</xdr:row>
       <xdr:rowOff>158750</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
       <xdr:colOff>482600</xdr:colOff>
-      <xdr:row>59</xdr:row>
+      <xdr:row>61</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -691,13 +700,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>228600</xdr:colOff>
-      <xdr:row>59</xdr:row>
+      <xdr:row>61</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
       <xdr:colOff>488950</xdr:colOff>
-      <xdr:row>60</xdr:row>
+      <xdr:row>62</xdr:row>
       <xdr:rowOff>44450</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -755,13 +764,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>260350</xdr:colOff>
-      <xdr:row>60</xdr:row>
+      <xdr:row>62</xdr:row>
       <xdr:rowOff>31750</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
       <xdr:colOff>400050</xdr:colOff>
-      <xdr:row>60</xdr:row>
+      <xdr:row>62</xdr:row>
       <xdr:rowOff>165100</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -815,13 +824,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>266700</xdr:colOff>
-      <xdr:row>61</xdr:row>
+      <xdr:row>63</xdr:row>
       <xdr:rowOff>31750</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
       <xdr:colOff>406400</xdr:colOff>
-      <xdr:row>61</xdr:row>
+      <xdr:row>63</xdr:row>
       <xdr:rowOff>165100</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -875,13 +884,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>260350</xdr:colOff>
-      <xdr:row>62</xdr:row>
+      <xdr:row>64</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
       <xdr:colOff>400050</xdr:colOff>
-      <xdr:row>62</xdr:row>
+      <xdr:row>64</xdr:row>
       <xdr:rowOff>171450</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1250,10 +1259,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:S63"/>
+  <dimension ref="A1:S65"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="S12" sqref="S12"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="L29" sqref="L29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1286,7 +1295,7 @@
         <v>40</v>
       </c>
       <c r="P1" s="66">
-        <f>C35</f>
+        <f>C37</f>
         <v>0.12</v>
       </c>
     </row>
@@ -1296,8 +1305,8 @@
         <v>41</v>
       </c>
       <c r="P2" s="66">
-        <f>C36</f>
-        <v>0.12</v>
+        <f>C38</f>
+        <v>0.17</v>
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
@@ -1306,7 +1315,7 @@
         <v>4</v>
       </c>
       <c r="P3" s="67">
-        <f>H30</f>
+        <f>H32</f>
         <v>1.6500000000000001E-2</v>
       </c>
     </row>
@@ -1316,7 +1325,7 @@
         <v>5</v>
       </c>
       <c r="P4" s="67">
-        <f>H29</f>
+        <f>H31</f>
         <v>7.5999999999999998E-2</v>
       </c>
     </row>
@@ -1326,7 +1335,7 @@
         <v>37</v>
       </c>
       <c r="P5" s="1">
-        <f>F15</f>
+        <f>F17</f>
         <v>1000</v>
       </c>
     </row>
@@ -1336,7 +1345,7 @@
         <v>38</v>
       </c>
       <c r="P6" s="1">
-        <f>F22</f>
+        <f>F24</f>
         <v>40000</v>
       </c>
     </row>
@@ -1400,14 +1409,14 @@
       </c>
       <c r="P11" s="76">
         <f>(P7-P13)</f>
-        <v>88000</v>
+        <v>83000</v>
       </c>
       <c r="R11" s="80" t="s">
         <v>4</v>
       </c>
       <c r="S11" s="81">
         <f>(P12*P3)-(O12*P3)</f>
-        <v>777.48</v>
+        <v>694.98</v>
       </c>
     </row>
     <row r="12" spans="1:19" ht="18.75" x14ac:dyDescent="0.3">
@@ -1429,14 +1438,14 @@
       </c>
       <c r="P12" s="79">
         <f>SUM(P11)</f>
-        <v>88000</v>
+        <v>83000</v>
       </c>
       <c r="R12" s="80" t="s">
         <v>5</v>
       </c>
       <c r="S12" s="81">
         <f>(P12*P4)-(O12*P4)</f>
-        <v>3581.12</v>
+        <v>3201.12</v>
       </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
@@ -1459,7 +1468,7 @@
       </c>
       <c r="P13" s="75">
         <f>P7*P2</f>
-        <v>12000</v>
+        <v>17000</v>
       </c>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
@@ -1480,484 +1489,518 @@
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B15" s="10" t="s">
-        <v>0</v>
+        <v>53</v>
       </c>
       <c r="F15" s="47">
-        <v>1000</v>
+        <v>3000</v>
       </c>
       <c r="G15" s="11">
-        <f>F15/$F$14</f>
-        <v>0.01</v>
+        <f t="shared" ref="G15:G16" si="0">F15/$F$14</f>
+        <v>0.03</v>
       </c>
       <c r="H15" s="18">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="J15" s="40"/>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B16" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="F16" s="47">
+        <v>4000</v>
+      </c>
+      <c r="G16" s="11">
+        <f t="shared" si="0"/>
+        <v>0.04</v>
+      </c>
+      <c r="H16" s="18">
+        <v>2</v>
+      </c>
+      <c r="J16" s="40"/>
+    </row>
+    <row r="17" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B17" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="F17" s="47">
+        <v>1000</v>
+      </c>
+      <c r="G17" s="11">
+        <f>F17/$F$14</f>
+        <v>0.01</v>
+      </c>
+      <c r="H17" s="18">
+        <v>5</v>
+      </c>
+      <c r="J17" s="40"/>
+    </row>
+    <row r="18" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B18" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="F16" s="47">
+      <c r="F18" s="47">
         <v>2000</v>
       </c>
-      <c r="G16" s="11">
-        <f>F16/$F$14</f>
+      <c r="G18" s="11">
+        <f>F18/$F$14</f>
         <v>0.02</v>
       </c>
-      <c r="H16" s="18">
+      <c r="H18" s="18">
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B17" s="10"/>
-      <c r="F17" s="46"/>
-      <c r="G17" s="11"/>
-      <c r="H17" s="12"/>
-    </row>
-    <row r="18" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B18" s="19" t="s">
+    <row r="19" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B19" s="10"/>
+      <c r="F19" s="46"/>
+      <c r="G19" s="11"/>
+      <c r="H19" s="12"/>
+    </row>
+    <row r="20" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B20" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="C18" s="35"/>
-      <c r="D18" s="35"/>
-      <c r="E18" s="35"/>
-      <c r="F18" s="50"/>
-      <c r="G18" s="20">
-        <f>SUM(G19:G20)</f>
+      <c r="C20" s="35"/>
+      <c r="D20" s="35"/>
+      <c r="E20" s="35"/>
+      <c r="F20" s="50"/>
+      <c r="G20" s="20">
+        <f>SUM(G21:G22)</f>
         <v>0.09</v>
       </c>
-      <c r="H18" s="21"/>
-      <c r="K18" s="62"/>
-      <c r="L18" s="47"/>
-      <c r="M18" s="62"/>
-      <c r="N18" s="62">
-        <f>+K18*L18</f>
+      <c r="H20" s="21"/>
+      <c r="K20" s="62"/>
+      <c r="L20" s="47"/>
+      <c r="M20" s="62"/>
+      <c r="N20" s="62">
+        <f>+K20*L20</f>
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B19" s="22" t="s">
+    <row r="21" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B21" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="F19" s="47">
+      <c r="F21" s="47">
         <v>9000</v>
       </c>
-      <c r="G19" s="23">
-        <f>F19/F14</f>
+      <c r="G21" s="23">
+        <f>F21/F14</f>
         <v>0.09</v>
       </c>
-      <c r="H19" s="64">
+      <c r="H21" s="64">
         <v>0.17</v>
       </c>
-      <c r="J19" s="3"/>
-      <c r="K19" s="62"/>
-      <c r="L19" s="47"/>
-      <c r="M19" s="62"/>
-      <c r="N19" s="62">
-        <f>SUM(N18:N18)</f>
+      <c r="J21" s="3"/>
+      <c r="K21" s="62"/>
+      <c r="L21" s="47"/>
+      <c r="M21" s="62"/>
+      <c r="N21" s="62">
+        <f>SUM(N20:N20)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B20" s="22"/>
-      <c r="F20" s="51"/>
-      <c r="G20" s="23"/>
-      <c r="H20" s="24"/>
-    </row>
-    <row r="21" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B21" s="19" t="s">
+    <row r="22" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B22" s="22"/>
+      <c r="F22" s="51"/>
+      <c r="G22" s="23"/>
+      <c r="H22" s="24"/>
+    </row>
+    <row r="23" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B23" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="C21" s="35"/>
-      <c r="D21" s="35"/>
-      <c r="E21" s="35"/>
-      <c r="F21" s="50"/>
-      <c r="G21" s="20"/>
-      <c r="H21" s="21"/>
-    </row>
-    <row r="22" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B22" s="10" t="s">
+      <c r="C23" s="35"/>
+      <c r="D23" s="35"/>
+      <c r="E23" s="35"/>
+      <c r="F23" s="50"/>
+      <c r="G23" s="20"/>
+      <c r="H23" s="21"/>
+    </row>
+    <row r="24" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B24" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="C22" s="48">
-        <f>F22/16</f>
+      <c r="C24" s="48">
+        <f>F24/16</f>
         <v>2500</v>
       </c>
-      <c r="D22" s="49" t="s">
+      <c r="D24" s="49" t="s">
         <v>26</v>
       </c>
-      <c r="F22" s="47">
-        <f>H22*F14</f>
+      <c r="F24" s="47">
+        <f>H24*F14</f>
         <v>40000</v>
       </c>
-      <c r="G22" s="11">
-        <f>F22/F14</f>
+      <c r="G24" s="11">
+        <f>F24/F14</f>
         <v>0.4</v>
       </c>
-      <c r="H22" s="65">
+      <c r="H24" s="65">
         <v>0.4</v>
       </c>
     </row>
-    <row r="23" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B23" s="10" t="s">
+    <row r="25" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B25" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="C23" s="48">
-        <f>F23/16</f>
+      <c r="C25" s="48">
+        <f>F25/16</f>
         <v>3000</v>
       </c>
-      <c r="D23" s="49" t="s">
+      <c r="D25" s="49" t="s">
         <v>26</v>
       </c>
-      <c r="F23" s="47">
-        <f>G23*F14</f>
+      <c r="F25" s="47">
+        <f>G25*F14</f>
         <v>48000</v>
       </c>
-      <c r="G23" s="11">
-        <f>(100%-SUM(G15:G17,G18,G22))</f>
+      <c r="G25" s="11">
+        <f>(100%-SUM(G17:G19,G20,G24))</f>
         <v>0.48</v>
       </c>
-      <c r="H23" s="12"/>
-    </row>
-    <row r="24" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="25" t="s">
+      <c r="H25" s="12"/>
+    </row>
+    <row r="26" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B26" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="C24" s="26"/>
-      <c r="D24" s="26"/>
-      <c r="E24" s="26"/>
-      <c r="F24" s="52"/>
-      <c r="G24" s="37">
-        <f>100% - SUM(G19:G20,G22:G23)</f>
+      <c r="C26" s="26"/>
+      <c r="D26" s="26"/>
+      <c r="E26" s="26"/>
+      <c r="F26" s="52"/>
+      <c r="G26" s="37">
+        <f>100% - SUM(G21:G22,G24:G25)</f>
         <v>3.0000000000000027E-2</v>
       </c>
-      <c r="H24" s="27"/>
-    </row>
-    <row r="25" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F25" s="1"/>
-      <c r="G25" s="4"/>
-    </row>
-    <row r="26" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B26" s="6" t="s">
+      <c r="H26" s="27"/>
+    </row>
+    <row r="27" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F27" s="1"/>
+      <c r="G27" s="4"/>
+    </row>
+    <row r="28" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B28" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C26" s="34"/>
-      <c r="D26" s="34"/>
-      <c r="E26" s="34"/>
-      <c r="F26" s="7"/>
-      <c r="G26" s="8"/>
-      <c r="H26" s="9"/>
-    </row>
-    <row r="27" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B27" s="10"/>
-      <c r="F27" s="1"/>
-      <c r="G27" s="28" t="s">
+      <c r="C28" s="34"/>
+      <c r="D28" s="34"/>
+      <c r="E28" s="34"/>
+      <c r="F28" s="7"/>
+      <c r="G28" s="8"/>
+      <c r="H28" s="9"/>
+    </row>
+    <row r="29" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B29" s="10"/>
+      <c r="F29" s="1"/>
+      <c r="G29" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="H27" s="12"/>
-    </row>
-    <row r="28" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B28" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="F28" s="47">
-        <f>F14*H28</f>
-        <v>1617.9207781519399</v>
-      </c>
-      <c r="G28" s="11">
-        <f>F28/F14</f>
-        <v>1.6179207781519399E-2</v>
-      </c>
-      <c r="H28" s="84">
-        <v>1.6179207781519399E-2</v>
-      </c>
-      <c r="L28" s="46"/>
-      <c r="O28" s="82"/>
-      <c r="P28" s="82"/>
-    </row>
-    <row r="29" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B29" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="F29" s="47">
-        <f>S12</f>
-        <v>3581.12</v>
-      </c>
-      <c r="G29" s="11">
-        <f>F29/$F$14</f>
-        <v>3.5811200000000001E-2</v>
-      </c>
-      <c r="H29" s="84">
-        <v>7.5999999999999998E-2</v>
-      </c>
-      <c r="L29" s="3"/>
-      <c r="O29" s="82"/>
-      <c r="P29" s="82"/>
+      <c r="H29" s="12"/>
     </row>
     <row r="30" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B30" s="10" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="F30" s="47">
-        <f>S11</f>
-        <v>777.48</v>
+        <f>F14*H30</f>
+        <v>1617.9207781519399</v>
       </c>
       <c r="G30" s="11">
-        <f t="shared" ref="G30:G33" si="0">F30/$F$14</f>
-        <v>7.7748000000000001E-3</v>
+        <f>F30/F14</f>
+        <v>1.6179207781519399E-2</v>
       </c>
       <c r="H30" s="84">
-        <v>1.6500000000000001E-2</v>
-      </c>
+        <v>1.6179207781519399E-2</v>
+      </c>
+      <c r="L30" s="46"/>
       <c r="O30" s="82"/>
       <c r="P30" s="82"/>
     </row>
     <row r="31" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B31" s="10" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="F31" s="47">
-        <f>IF(F23&gt;0,F23*H31,0)</f>
-        <v>7200</v>
+        <f>S12</f>
+        <v>3201.12</v>
       </c>
       <c r="G31" s="11">
-        <f t="shared" si="0"/>
-        <v>7.1999999999999995E-2</v>
+        <f>F31/$F$14</f>
+        <v>3.2011199999999997E-2</v>
       </c>
       <c r="H31" s="84">
-        <v>0.15</v>
-      </c>
+        <v>7.5999999999999998E-2</v>
+      </c>
+      <c r="L31" s="3"/>
       <c r="O31" s="82"/>
       <c r="P31" s="82"/>
     </row>
     <row r="32" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B32" s="10" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="F32" s="47">
-        <f>IF(F23&gt;0,F23*H32,0)</f>
-        <v>4320</v>
+        <f>S11</f>
+        <v>694.98</v>
       </c>
       <c r="G32" s="11">
-        <f t="shared" si="0"/>
-        <v>4.3200000000000002E-2</v>
+        <f t="shared" ref="G32:G35" si="1">F32/$F$14</f>
+        <v>6.9497999999999999E-3</v>
       </c>
       <c r="H32" s="84">
-        <v>0.09</v>
+        <v>1.6500000000000001E-2</v>
       </c>
       <c r="O32" s="82"/>
       <c r="P32" s="82"/>
     </row>
-    <row r="33" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B33" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="F33" s="47">
+        <f>IF(F25&gt;0,F25*H33,0)</f>
+        <v>7200</v>
+      </c>
+      <c r="G33" s="11">
+        <f t="shared" si="1"/>
+        <v>7.1999999999999995E-2</v>
+      </c>
+      <c r="H33" s="84">
+        <v>0.15</v>
+      </c>
+      <c r="O33" s="82"/>
+      <c r="P33" s="82"/>
+    </row>
+    <row r="34" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B34" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="F34" s="47">
+        <f>IF(F25&gt;0,F25*H34,0)</f>
+        <v>4320</v>
+      </c>
+      <c r="G34" s="11">
+        <f t="shared" si="1"/>
+        <v>4.3200000000000002E-2</v>
+      </c>
+      <c r="H34" s="84">
+        <v>0.09</v>
+      </c>
+      <c r="O34" s="82"/>
+      <c r="P34" s="82"/>
+    </row>
+    <row r="35" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B35" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="F33" s="47">
-        <f>+(H33*F14)-(F15*12%)</f>
+      <c r="F35" s="47">
+        <f>+(H35*F14)-(F17*12%)</f>
         <v>11880</v>
       </c>
-      <c r="G33" s="11">
-        <f t="shared" si="0"/>
+      <c r="G35" s="11">
+        <f t="shared" si="1"/>
         <v>0.1188</v>
       </c>
-      <c r="H33" s="84">
+      <c r="H35" s="84">
         <v>0.12</v>
       </c>
-      <c r="J33" s="4"/>
-    </row>
-    <row r="34" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B34" s="10"/>
-      <c r="F34" s="1"/>
-      <c r="G34" s="11"/>
-      <c r="H34" s="12"/>
-      <c r="J34" s="4"/>
-    </row>
-    <row r="35" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B35" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="C35" s="66">
-        <v>0.12</v>
-      </c>
-      <c r="F35" s="1"/>
-      <c r="G35" s="11"/>
-      <c r="H35" s="12"/>
-    </row>
-    <row r="36" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B36" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="C36" s="66">
-        <v>0.12</v>
-      </c>
+      <c r="J35" s="4"/>
+    </row>
+    <row r="36" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B36" s="10"/>
       <c r="F36" s="1"/>
       <c r="G36" s="11"/>
       <c r="H36" s="12"/>
-    </row>
-    <row r="37" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B37" s="10"/>
+      <c r="J36" s="4" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="37" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B37" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="C37" s="66">
+        <v>0.12</v>
+      </c>
       <c r="F37" s="1"/>
       <c r="G37" s="11"/>
       <c r="H37" s="12"/>
     </row>
-    <row r="38" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B38" s="10"/>
+    <row r="38" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B38" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="C38" s="66">
+        <v>0.17</v>
+      </c>
       <c r="F38" s="1"/>
       <c r="G38" s="11"/>
       <c r="H38" s="12"/>
     </row>
-    <row r="39" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B39" s="42" t="s">
+    <row r="39" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B39" s="10"/>
+      <c r="F39" s="1"/>
+      <c r="G39" s="11"/>
+      <c r="H39" s="12"/>
+    </row>
+    <row r="40" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B40" s="10"/>
+      <c r="F40" s="1"/>
+      <c r="G40" s="11"/>
+      <c r="H40" s="12"/>
+    </row>
+    <row r="41" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B41" s="42" t="s">
         <v>8</v>
       </c>
-      <c r="C39" s="43"/>
-      <c r="D39" s="43"/>
-      <c r="E39" s="43"/>
-      <c r="F39" s="61">
-        <f>SUM(F28:F38)</f>
-        <v>29376.520778151942</v>
-      </c>
-      <c r="G39" s="44">
-        <f>G28+G31+G32+G33+G29+G30+G34</f>
-        <v>0.29376520778151943</v>
-      </c>
-      <c r="H39" s="45"/>
-    </row>
-    <row r="40" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B40" s="53"/>
-      <c r="C40" s="53"/>
-      <c r="D40" s="53"/>
-      <c r="E40" s="53"/>
-      <c r="F40" s="54"/>
-      <c r="G40" s="55"/>
-      <c r="H40" s="53"/>
-    </row>
-    <row r="41" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B41" s="56" t="s">
+      <c r="C41" s="43"/>
+      <c r="D41" s="43"/>
+      <c r="E41" s="43"/>
+      <c r="F41" s="61">
+        <f>SUM(F30:F40)</f>
+        <v>28914.020778151942</v>
+      </c>
+      <c r="G41" s="44">
+        <f>G30+G33+G34+G35+G31+G32+G36</f>
+        <v>0.28914020778151944</v>
+      </c>
+      <c r="H41" s="45"/>
+    </row>
+    <row r="42" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B42" s="53"/>
+      <c r="C42" s="53"/>
+      <c r="D42" s="53"/>
+      <c r="E42" s="53"/>
+      <c r="F42" s="54"/>
+      <c r="G42" s="55"/>
+      <c r="H42" s="53"/>
+    </row>
+    <row r="43" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B43" s="56" t="s">
         <v>16</v>
       </c>
-      <c r="C41" s="57"/>
-      <c r="D41" s="57"/>
-      <c r="E41" s="57"/>
-      <c r="F41" s="58"/>
-      <c r="G41" s="59"/>
-      <c r="H41" s="60"/>
-    </row>
-    <row r="42" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B42" s="10" t="s">
+      <c r="C43" s="57"/>
+      <c r="D43" s="57"/>
+      <c r="E43" s="57"/>
+      <c r="F43" s="58"/>
+      <c r="G43" s="59"/>
+      <c r="H43" s="60"/>
+    </row>
+    <row r="44" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B44" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="G42" s="1" t="s">
+      <c r="G44" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="H42" s="12"/>
-    </row>
-    <row r="43" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B43" s="10" t="s">
+      <c r="H44" s="12"/>
+    </row>
+    <row r="45" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B45" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="G43" s="1" t="s">
+      <c r="G45" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="H43" s="12"/>
-    </row>
-    <row r="44" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B44" s="10" t="s">
+      <c r="H45" s="12"/>
+    </row>
+    <row r="46" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B46" s="10" t="s">
         <v>17</v>
-      </c>
-      <c r="G44" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H44" s="12"/>
-    </row>
-    <row r="45" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B45" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="G45" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H45" s="12"/>
-    </row>
-    <row r="46" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B46" s="10" t="s">
-        <v>4</v>
       </c>
       <c r="G46" s="1" t="s">
         <v>14</v>
       </c>
       <c r="H46" s="12"/>
     </row>
-    <row r="47" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B47" s="29" t="s">
+    <row r="47" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B47" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="G47" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H47" s="12"/>
+    </row>
+    <row r="48" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B48" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="G48" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H48" s="12"/>
+    </row>
+    <row r="49" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B49" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="C47" s="30"/>
-      <c r="D47" s="30"/>
-      <c r="E47" s="30"/>
-      <c r="F47" s="30"/>
-      <c r="G47" s="31" t="s">
+      <c r="C49" s="30"/>
+      <c r="D49" s="30"/>
+      <c r="E49" s="30"/>
+      <c r="F49" s="30"/>
+      <c r="G49" s="31" t="s">
         <v>14</v>
       </c>
-      <c r="H47" s="32"/>
-    </row>
-    <row r="49" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C49" s="1"/>
-      <c r="D49" s="4"/>
-    </row>
-    <row r="50" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C50" s="1"/>
-      <c r="D50" s="4"/>
-    </row>
-    <row r="51" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="H49" s="32"/>
+    </row>
+    <row r="51" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C51" s="1"/>
       <c r="D51" s="4"/>
     </row>
-    <row r="52" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C52" s="1"/>
       <c r="D52" s="4"/>
     </row>
-    <row r="57" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B57" s="86" t="s">
+    <row r="53" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C53" s="1"/>
+      <c r="D53" s="4"/>
+    </row>
+    <row r="54" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C54" s="1"/>
+      <c r="D54" s="4"/>
+    </row>
+    <row r="59" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B59" s="86" t="s">
         <v>7</v>
       </c>
-      <c r="C57" s="86"/>
-    </row>
-    <row r="58" spans="2:4" ht="11.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B58" t="s">
+      <c r="C59" s="86"/>
+    </row>
+    <row r="60" spans="2:8" ht="11.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B60" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="59" spans="2:4" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B59" t="s">
+    <row r="61" spans="2:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B61" t="s">
         <v>1</v>
       </c>
-      <c r="C59" s="5"/>
-    </row>
-    <row r="60" spans="2:4" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B60" t="s">
+      <c r="C61" s="5"/>
+    </row>
+    <row r="62" spans="2:8" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B62" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="61" spans="2:4" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B61" t="s">
+    <row r="63" spans="2:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B63" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="62" spans="2:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B62" t="s">
+    <row r="64" spans="2:8" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B64" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="63" spans="2:4" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B63" t="s">
+    <row r="65" spans="2:2" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B65" t="s">
         <v>5</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="B57:C57"/>
+    <mergeCell ref="B59:C59"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" scale="39" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
feat - ajustes nos testes de gerar resumo_tributario
</commit_message>
<xml_diff>
--- a/template.xlsx
+++ b/template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luan\Documents\Projetos\Entercap\ENTERCAP-Resumo-tributario\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11D44A26-CC3E-4EC2-9E73-0DACF2DF7001}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0199EAF4-A20C-4F95-919F-AB25A705BD53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1262,7 +1262,7 @@
   <dimension ref="A1:S65"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A5" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="L29" sqref="L29"/>
+      <selection activeCell="F35" sqref="F35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1589,6 +1589,7 @@
         <v>0.09</v>
       </c>
       <c r="H21" s="64">
+        <f>C38</f>
         <v>0.17</v>
       </c>
       <c r="J21" s="3"/>
@@ -1703,7 +1704,7 @@
         <v>25</v>
       </c>
       <c r="F30" s="47">
-        <f>F14*H30</f>
+        <f>$F$14*H30</f>
         <v>1617.9207781519399</v>
       </c>
       <c r="G30" s="11">
@@ -1799,7 +1800,7 @@
         <v>11880</v>
       </c>
       <c r="G35" s="11">
-        <f t="shared" si="1"/>
+        <f>F35/$F$14</f>
         <v>0.1188</v>
       </c>
       <c r="H35" s="84">
@@ -1858,7 +1859,7 @@
       <c r="D41" s="43"/>
       <c r="E41" s="43"/>
       <c r="F41" s="61">
-        <f>SUM(F30:F40)</f>
+        <f>SUM(F29:F40)</f>
         <v>28914.020778151942</v>
       </c>
       <c r="G41" s="44">

</xml_diff>

<commit_message>
feat - icms agora fica icms mensal - template nao tem mais linhas em branco - icms dif al aba apresentação
</commit_message>
<xml_diff>
--- a/template.xlsx
+++ b/template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luan\Documents\Projetos\Entercap\ENTERCAP-Resumo-tributario\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0199EAF4-A20C-4F95-919F-AB25A705BD53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25167A7F-5406-43DF-AFCC-405216720451}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="57">
   <si>
     <t>COMPRAS</t>
   </si>
@@ -207,6 +207,9 @@
   </si>
   <si>
     <t>b</t>
+  </si>
+  <si>
+    <t>ICMS Mensal</t>
   </si>
 </sst>
 </file>
@@ -490,7 +493,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="87">
+  <cellXfs count="86">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
@@ -519,9 +522,6 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="3" fillId="3" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="3" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
@@ -560,9 +560,6 @@
     <xf numFmtId="4" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="4" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -581,7 +578,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -607,6 +603,12 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="1" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -636,13 +638,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>222250</xdr:colOff>
-      <xdr:row>59</xdr:row>
+      <xdr:row>57</xdr:row>
       <xdr:rowOff>158750</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
       <xdr:colOff>482600</xdr:colOff>
-      <xdr:row>61</xdr:row>
+      <xdr:row>59</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -700,13 +702,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>228600</xdr:colOff>
-      <xdr:row>61</xdr:row>
+      <xdr:row>59</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
       <xdr:colOff>488950</xdr:colOff>
-      <xdr:row>62</xdr:row>
+      <xdr:row>60</xdr:row>
       <xdr:rowOff>44450</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -764,13 +766,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>260350</xdr:colOff>
-      <xdr:row>62</xdr:row>
+      <xdr:row>60</xdr:row>
       <xdr:rowOff>31750</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
       <xdr:colOff>400050</xdr:colOff>
-      <xdr:row>62</xdr:row>
+      <xdr:row>60</xdr:row>
       <xdr:rowOff>165100</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -824,13 +826,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>266700</xdr:colOff>
-      <xdr:row>63</xdr:row>
+      <xdr:row>61</xdr:row>
       <xdr:rowOff>31750</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
       <xdr:colOff>406400</xdr:colOff>
-      <xdr:row>63</xdr:row>
+      <xdr:row>61</xdr:row>
       <xdr:rowOff>165100</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -884,13 +886,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>260350</xdr:colOff>
-      <xdr:row>64</xdr:row>
+      <xdr:row>62</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
       <xdr:colOff>400050</xdr:colOff>
-      <xdr:row>64</xdr:row>
+      <xdr:row>62</xdr:row>
       <xdr:rowOff>171450</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1259,10 +1261,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:S65"/>
+  <dimension ref="A1:S63"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A5" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="F35" sqref="F35"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1274,12 +1276,12 @@
     <col min="6" max="6" width="16.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13.5703125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10.5703125" customWidth="1"/>
-    <col min="9" max="9" width="8.85546875" style="39"/>
+    <col min="9" max="9" width="8.85546875" style="36"/>
     <col min="10" max="10" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.7109375" style="49"/>
+    <col min="11" max="11" width="8.7109375" style="46"/>
     <col min="12" max="12" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="2.85546875" style="49" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="19.140625" style="49" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="2.85546875" style="46" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="19.140625" style="46" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="14.5703125" customWidth="1"/>
     <col min="16" max="16" width="14.5703125" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="7.85546875" bestFit="1" customWidth="1"/>
@@ -1294,8 +1296,8 @@
       <c r="O1" t="s">
         <v>40</v>
       </c>
-      <c r="P1" s="66">
-        <f>C37</f>
+      <c r="P1" s="61">
+        <f>C35</f>
         <v>0.12</v>
       </c>
     </row>
@@ -1304,8 +1306,8 @@
       <c r="O2" t="s">
         <v>41</v>
       </c>
-      <c r="P2" s="66">
-        <f>C38</f>
+      <c r="P2" s="61">
+        <f>C36</f>
         <v>0.17</v>
       </c>
     </row>
@@ -1314,8 +1316,8 @@
       <c r="O3" t="s">
         <v>4</v>
       </c>
-      <c r="P3" s="67">
-        <f>H32</f>
+      <c r="P3" s="62">
+        <f>H30</f>
         <v>1.6500000000000001E-2</v>
       </c>
     </row>
@@ -1324,8 +1326,8 @@
       <c r="O4" t="s">
         <v>5</v>
       </c>
-      <c r="P4" s="67">
-        <f>H31</f>
+      <c r="P4" s="62">
+        <f>H29</f>
         <v>7.5999999999999998E-2</v>
       </c>
     </row>
@@ -1345,19 +1347,19 @@
         <v>38</v>
       </c>
       <c r="P6" s="1">
-        <f>F24</f>
+        <f>F22</f>
         <v>40000</v>
       </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A7" s="41"/>
-      <c r="B7" s="38" t="s">
+      <c r="A7" s="38"/>
+      <c r="B7" s="35" t="s">
         <v>50</v>
       </c>
-      <c r="C7" s="83" t="s">
+      <c r="C7" s="78" t="s">
         <v>51</v>
       </c>
-      <c r="D7" s="41"/>
+      <c r="D7" s="38"/>
       <c r="H7" s="2"/>
       <c r="N7"/>
       <c r="O7" t="s">
@@ -1369,52 +1371,52 @@
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="N8" s="68"/>
-      <c r="O8" s="69" t="s">
+      <c r="N8" s="63"/>
+      <c r="O8" s="64" t="s">
         <v>35</v>
       </c>
-      <c r="P8" s="70" t="s">
+      <c r="P8" s="65" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="N9" s="71" t="s">
+      <c r="N9" s="66" t="s">
         <v>42</v>
       </c>
-      <c r="O9" s="63">
+      <c r="O9" s="59">
         <f>(P5-O13)</f>
         <v>880</v>
       </c>
-      <c r="P9" s="72"/>
+      <c r="P9" s="67"/>
     </row>
     <row r="10" spans="1:19" ht="21" x14ac:dyDescent="0.35">
-      <c r="B10" s="33" t="s">
+      <c r="B10" s="30" t="s">
         <v>49</v>
       </c>
       <c r="C10" t="s">
         <v>34</v>
       </c>
-      <c r="N10" s="71" t="s">
+      <c r="N10" s="66" t="s">
         <v>43</v>
       </c>
       <c r="O10" s="1">
         <f>P6</f>
         <v>40000</v>
       </c>
-      <c r="P10" s="72"/>
+      <c r="P10" s="67"/>
     </row>
     <row r="11" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="N11" s="71" t="s">
+      <c r="N11" s="66" t="s">
         <v>44</v>
       </c>
-      <c r="P11" s="76">
+      <c r="P11" s="71">
         <f>(P7-P13)</f>
         <v>83000</v>
       </c>
-      <c r="R11" s="80" t="s">
+      <c r="R11" s="75" t="s">
         <v>4</v>
       </c>
-      <c r="S11" s="81">
+      <c r="S11" s="76">
         <f>(P12*P3)-(O12*P3)</f>
         <v>694.98</v>
       </c>
@@ -1423,27 +1425,27 @@
       <c r="B12" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="C12" s="36"/>
-      <c r="D12" s="36"/>
-      <c r="E12" s="36"/>
+      <c r="C12" s="33"/>
+      <c r="D12" s="33"/>
+      <c r="E12" s="33"/>
       <c r="F12" s="14"/>
       <c r="G12" s="14"/>
       <c r="H12" s="15"/>
-      <c r="N12" s="77" t="s">
+      <c r="N12" s="72" t="s">
         <v>46</v>
       </c>
-      <c r="O12" s="78">
+      <c r="O12" s="73">
         <f>SUM(O9:O11)</f>
         <v>40880</v>
       </c>
-      <c r="P12" s="79">
+      <c r="P12" s="74">
         <f>SUM(P11)</f>
         <v>83000</v>
       </c>
-      <c r="R12" s="80" t="s">
+      <c r="R12" s="75" t="s">
         <v>5</v>
       </c>
-      <c r="S12" s="81">
+      <c r="S12" s="76">
         <f>(P12*P4)-(O12*P4)</f>
         <v>3201.12</v>
       </c>
@@ -1459,14 +1461,14 @@
       <c r="H13" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="N13" s="73" t="s">
+      <c r="N13" s="68" t="s">
         <v>45</v>
       </c>
-      <c r="O13" s="74">
+      <c r="O13" s="69">
         <f>P5*P1</f>
         <v>120</v>
       </c>
-      <c r="P13" s="75">
+      <c r="P13" s="70">
         <f>P7*P2</f>
         <v>17000</v>
       </c>
@@ -1475,7 +1477,7 @@
       <c r="B14" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="F14" s="47">
+      <c r="F14" s="44">
         <v>100000</v>
       </c>
       <c r="G14" s="11">
@@ -1485,13 +1487,13 @@
       <c r="H14" s="18">
         <v>5</v>
       </c>
-      <c r="J14" s="40"/>
+      <c r="J14" s="37"/>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B15" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="F15" s="47">
+      <c r="F15" s="44">
         <v>3000</v>
       </c>
       <c r="G15" s="11">
@@ -1501,13 +1503,13 @@
       <c r="H15" s="18">
         <v>1</v>
       </c>
-      <c r="J15" s="40"/>
+      <c r="J15" s="37"/>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B16" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="F16" s="47">
+      <c r="F16" s="44">
         <v>4000</v>
       </c>
       <c r="G16" s="11">
@@ -1517,13 +1519,13 @@
       <c r="H16" s="18">
         <v>2</v>
       </c>
-      <c r="J16" s="40"/>
+      <c r="J16" s="37"/>
     </row>
     <row r="17" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B17" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="F17" s="47">
+      <c r="F17" s="44">
         <v>1000</v>
       </c>
       <c r="G17" s="11">
@@ -1533,13 +1535,13 @@
       <c r="H17" s="18">
         <v>5</v>
       </c>
-      <c r="J17" s="40"/>
+      <c r="J17" s="37"/>
     </row>
     <row r="18" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B18" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="F18" s="47">
+      <c r="F18" s="44">
         <v>2000</v>
       </c>
       <c r="G18" s="11">
@@ -1551,457 +1553,429 @@
       </c>
     </row>
     <row r="19" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B19" s="10"/>
-      <c r="F19" s="46"/>
-      <c r="G19" s="11"/>
-      <c r="H19" s="12"/>
+      <c r="B19" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="C19" s="32"/>
+      <c r="D19" s="32"/>
+      <c r="E19" s="32"/>
+      <c r="F19" s="47"/>
+      <c r="G19" s="20">
+        <f>SUM(G20:G20)</f>
+        <v>0</v>
+      </c>
+      <c r="H19" s="21"/>
+      <c r="K19" s="58"/>
+      <c r="L19" s="44"/>
+      <c r="M19" s="58"/>
+      <c r="N19" s="58">
+        <f>+K19*L19</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="20" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B20" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="C20" s="35"/>
-      <c r="D20" s="35"/>
-      <c r="E20" s="35"/>
-      <c r="F20" s="50"/>
-      <c r="G20" s="20">
-        <f>SUM(G21:G22)</f>
-        <v>0.09</v>
-      </c>
-      <c r="H20" s="21"/>
-      <c r="K20" s="62"/>
-      <c r="L20" s="47"/>
-      <c r="M20" s="62"/>
-      <c r="N20" s="62">
-        <f>+K20*L20</f>
-        <v>0</v>
-      </c>
+      <c r="B20" s="81" t="s">
+        <v>56</v>
+      </c>
+      <c r="F20" s="82"/>
+      <c r="G20" s="83"/>
+      <c r="H20" s="84"/>
     </row>
     <row r="21" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B21" s="22" t="s">
-        <v>2</v>
-      </c>
-      <c r="F21" s="47">
-        <v>9000</v>
-      </c>
-      <c r="G21" s="23">
-        <f>F21/F14</f>
-        <v>0.09</v>
-      </c>
-      <c r="H21" s="64">
-        <f>C38</f>
-        <v>0.17</v>
-      </c>
-      <c r="J21" s="3"/>
-      <c r="K21" s="62"/>
-      <c r="L21" s="47"/>
-      <c r="M21" s="62"/>
-      <c r="N21" s="62">
-        <f>SUM(N20:N20)</f>
-        <v>0</v>
-      </c>
+      <c r="B21" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="C21" s="32"/>
+      <c r="D21" s="32"/>
+      <c r="E21" s="32"/>
+      <c r="F21" s="47"/>
+      <c r="G21" s="20"/>
+      <c r="H21" s="21"/>
     </row>
     <row r="22" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B22" s="22"/>
-      <c r="F22" s="51"/>
-      <c r="G22" s="23"/>
-      <c r="H22" s="24"/>
+      <c r="B22" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C22" s="45">
+        <f>F22/16</f>
+        <v>2500</v>
+      </c>
+      <c r="D22" s="46" t="s">
+        <v>26</v>
+      </c>
+      <c r="F22" s="44">
+        <f>H22*F14</f>
+        <v>40000</v>
+      </c>
+      <c r="G22" s="11">
+        <f>F22/F14</f>
+        <v>0.4</v>
+      </c>
+      <c r="H22" s="60">
+        <v>0.4</v>
+      </c>
     </row>
     <row r="23" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B23" s="19" t="s">
-        <v>23</v>
-      </c>
-      <c r="C23" s="35"/>
-      <c r="D23" s="35"/>
-      <c r="E23" s="35"/>
-      <c r="F23" s="50"/>
-      <c r="G23" s="20"/>
-      <c r="H23" s="21"/>
-    </row>
-    <row r="24" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B24" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="C24" s="48">
-        <f>F24/16</f>
-        <v>2500</v>
-      </c>
-      <c r="D24" s="49" t="s">
+      <c r="B23" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="C23" s="45">
+        <f>F23/16</f>
+        <v>3562.4999999999995</v>
+      </c>
+      <c r="D23" s="46" t="s">
         <v>26</v>
       </c>
-      <c r="F24" s="47">
-        <f>H24*F14</f>
-        <v>40000</v>
-      </c>
-      <c r="G24" s="11">
-        <f>F24/F14</f>
-        <v>0.4</v>
-      </c>
-      <c r="H24" s="65">
-        <v>0.4</v>
-      </c>
-    </row>
-    <row r="25" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B25" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="C25" s="48">
-        <f>F25/16</f>
-        <v>3000</v>
-      </c>
-      <c r="D25" s="49" t="s">
-        <v>26</v>
-      </c>
-      <c r="F25" s="47">
-        <f>G25*F14</f>
-        <v>48000</v>
-      </c>
-      <c r="G25" s="11">
-        <f>(100%-SUM(G17:G19,G20,G24))</f>
-        <v>0.48</v>
-      </c>
-      <c r="H25" s="12"/>
-    </row>
-    <row r="26" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="25" t="s">
+      <c r="F23" s="44">
+        <f>G23*F14</f>
+        <v>56999.999999999993</v>
+      </c>
+      <c r="G23" s="11">
+        <f>(100%-SUM(G17:G18,G19,G22))</f>
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="H23" s="12"/>
+    </row>
+    <row r="24" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B24" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="C26" s="26"/>
-      <c r="D26" s="26"/>
-      <c r="E26" s="26"/>
-      <c r="F26" s="52"/>
-      <c r="G26" s="37">
-        <f>100% - SUM(G21:G22,G24:G25)</f>
+      <c r="C24" s="23"/>
+      <c r="D24" s="23"/>
+      <c r="E24" s="23"/>
+      <c r="F24" s="48"/>
+      <c r="G24" s="34">
+        <f>100% - SUM(G20:G20,G22:G23)</f>
         <v>3.0000000000000027E-2</v>
       </c>
-      <c r="H26" s="27"/>
-    </row>
-    <row r="27" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H24" s="24"/>
+    </row>
+    <row r="25" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F25" s="1"/>
+      <c r="G25" s="4"/>
+    </row>
+    <row r="26" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B26" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C26" s="31"/>
+      <c r="D26" s="31"/>
+      <c r="E26" s="31"/>
+      <c r="F26" s="7"/>
+      <c r="G26" s="8"/>
+      <c r="H26" s="9"/>
+    </row>
+    <row r="27" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B27" s="10"/>
       <c r="F27" s="1"/>
-      <c r="G27" s="4"/>
+      <c r="G27" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="H27" s="12"/>
     </row>
     <row r="28" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B28" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C28" s="34"/>
-      <c r="D28" s="34"/>
-      <c r="E28" s="34"/>
-      <c r="F28" s="7"/>
-      <c r="G28" s="8"/>
-      <c r="H28" s="9"/>
+      <c r="B28" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="F28" s="44">
+        <f>$F$14*H28</f>
+        <v>1617.9207781519399</v>
+      </c>
+      <c r="G28" s="11">
+        <f>F28/F14</f>
+        <v>1.6179207781519399E-2</v>
+      </c>
+      <c r="H28" s="79">
+        <v>1.6179207781519399E-2</v>
+      </c>
+      <c r="L28" s="43"/>
+      <c r="O28" s="77"/>
+      <c r="P28" s="77"/>
     </row>
     <row r="29" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B29" s="10"/>
-      <c r="F29" s="1"/>
-      <c r="G29" s="28" t="s">
-        <v>11</v>
-      </c>
-      <c r="H29" s="12"/>
+      <c r="B29" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="F29" s="44">
+        <f>S12</f>
+        <v>3201.12</v>
+      </c>
+      <c r="G29" s="11">
+        <f>F29/$F$14</f>
+        <v>3.2011199999999997E-2</v>
+      </c>
+      <c r="H29" s="79">
+        <v>7.5999999999999998E-2</v>
+      </c>
+      <c r="L29" s="3"/>
+      <c r="O29" s="77"/>
+      <c r="P29" s="77"/>
     </row>
     <row r="30" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B30" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="F30" s="47">
-        <f>$F$14*H30</f>
-        <v>1617.9207781519399</v>
+        <v>32</v>
+      </c>
+      <c r="F30" s="44">
+        <f>S11</f>
+        <v>694.98</v>
       </c>
       <c r="G30" s="11">
-        <f>F30/F14</f>
-        <v>1.6179207781519399E-2</v>
-      </c>
-      <c r="H30" s="84">
-        <v>1.6179207781519399E-2</v>
-      </c>
-      <c r="L30" s="46"/>
-      <c r="O30" s="82"/>
-      <c r="P30" s="82"/>
+        <f t="shared" ref="G30:G32" si="1">F30/$F$14</f>
+        <v>6.9497999999999999E-3</v>
+      </c>
+      <c r="H30" s="79">
+        <v>1.6500000000000001E-2</v>
+      </c>
+      <c r="O30" s="77"/>
+      <c r="P30" s="77"/>
     </row>
     <row r="31" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B31" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="F31" s="47">
-        <f>S12</f>
-        <v>3201.12</v>
+        <v>29</v>
+      </c>
+      <c r="F31" s="44">
+        <f>IF(F23&gt;0,F23*H31,0)</f>
+        <v>8549.9999999999982</v>
       </c>
       <c r="G31" s="11">
-        <f>F31/$F$14</f>
-        <v>3.2011199999999997E-2</v>
-      </c>
-      <c r="H31" s="84">
-        <v>7.5999999999999998E-2</v>
-      </c>
-      <c r="L31" s="3"/>
-      <c r="O31" s="82"/>
-      <c r="P31" s="82"/>
+        <f t="shared" si="1"/>
+        <v>8.5499999999999979E-2</v>
+      </c>
+      <c r="H31" s="79">
+        <v>0.15</v>
+      </c>
+      <c r="O31" s="77"/>
+      <c r="P31" s="77"/>
     </row>
     <row r="32" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B32" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="F32" s="47">
-        <f>S11</f>
-        <v>694.98</v>
+        <v>30</v>
+      </c>
+      <c r="F32" s="44">
+        <f>IF(F23&gt;0,F23*H32,0)</f>
+        <v>5129.9999999999991</v>
       </c>
       <c r="G32" s="11">
-        <f t="shared" ref="G32:G35" si="1">F32/$F$14</f>
-        <v>6.9497999999999999E-3</v>
-      </c>
-      <c r="H32" s="84">
-        <v>1.6500000000000001E-2</v>
-      </c>
-      <c r="O32" s="82"/>
-      <c r="P32" s="82"/>
-    </row>
-    <row r="33" spans="2:16" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>5.1299999999999991E-2</v>
+      </c>
+      <c r="H32" s="79">
+        <v>0.09</v>
+      </c>
+      <c r="O32" s="77"/>
+      <c r="P32" s="77"/>
+    </row>
+    <row r="33" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B33" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="F33" s="47">
-        <f>IF(F25&gt;0,F25*H33,0)</f>
-        <v>7200</v>
+        <v>2</v>
+      </c>
+      <c r="F33" s="44">
+        <f>+(H33*F14)-(F17*12%)</f>
+        <v>11880</v>
       </c>
       <c r="G33" s="11">
-        <f t="shared" si="1"/>
-        <v>7.1999999999999995E-2</v>
-      </c>
-      <c r="H33" s="84">
-        <v>0.15</v>
-      </c>
-      <c r="O33" s="82"/>
-      <c r="P33" s="82"/>
-    </row>
-    <row r="34" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B34" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="F34" s="47">
-        <f>IF(F25&gt;0,F25*H34,0)</f>
-        <v>4320</v>
-      </c>
-      <c r="G34" s="11">
-        <f t="shared" si="1"/>
-        <v>4.3200000000000002E-2</v>
-      </c>
-      <c r="H34" s="84">
-        <v>0.09</v>
-      </c>
-      <c r="O34" s="82"/>
-      <c r="P34" s="82"/>
-    </row>
-    <row r="35" spans="2:16" x14ac:dyDescent="0.25">
+        <f>F33/$F$14</f>
+        <v>0.1188</v>
+      </c>
+      <c r="H33" s="79">
+        <v>0.12</v>
+      </c>
+      <c r="J33" s="4"/>
+    </row>
+    <row r="34" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B34" s="10"/>
+      <c r="F34" s="1"/>
+      <c r="G34" s="11"/>
+      <c r="H34" s="12"/>
+      <c r="J34" s="4" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="35" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B35" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="F35" s="47">
-        <f>+(H35*F14)-(F17*12%)</f>
-        <v>11880</v>
-      </c>
-      <c r="G35" s="11">
-        <f>F35/$F$14</f>
-        <v>0.1188</v>
-      </c>
-      <c r="H35" s="84">
+        <v>47</v>
+      </c>
+      <c r="C35" s="61">
         <v>0.12</v>
       </c>
-      <c r="J35" s="4"/>
-    </row>
-    <row r="36" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B36" s="10"/>
+      <c r="F35" s="1"/>
+      <c r="G35" s="11"/>
+      <c r="H35" s="12"/>
+    </row>
+    <row r="36" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B36" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="C36" s="61">
+        <v>0.17</v>
+      </c>
       <c r="F36" s="1"/>
       <c r="G36" s="11"/>
       <c r="H36" s="12"/>
-      <c r="J36" s="4" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="37" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B37" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="C37" s="66">
-        <v>0.12</v>
-      </c>
+    </row>
+    <row r="37" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B37" s="10"/>
       <c r="F37" s="1"/>
       <c r="G37" s="11"/>
       <c r="H37" s="12"/>
     </row>
-    <row r="38" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B38" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="C38" s="66">
-        <v>0.17</v>
-      </c>
+    <row r="38" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B38" s="10"/>
       <c r="F38" s="1"/>
       <c r="G38" s="11"/>
       <c r="H38" s="12"/>
     </row>
-    <row r="39" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B39" s="10"/>
-      <c r="F39" s="1"/>
-      <c r="G39" s="11"/>
-      <c r="H39" s="12"/>
-    </row>
-    <row r="40" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B40" s="10"/>
-      <c r="F40" s="1"/>
-      <c r="G40" s="11"/>
-      <c r="H40" s="12"/>
-    </row>
-    <row r="41" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B41" s="42" t="s">
+    <row r="39" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B39" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="C41" s="43"/>
-      <c r="D41" s="43"/>
-      <c r="E41" s="43"/>
-      <c r="F41" s="61">
-        <f>SUM(F29:F40)</f>
-        <v>28914.020778151942</v>
-      </c>
-      <c r="G41" s="44">
-        <f>G30+G33+G34+G35+G31+G32+G36</f>
-        <v>0.28914020778151944</v>
-      </c>
-      <c r="H41" s="45"/>
-    </row>
-    <row r="42" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B42" s="53"/>
-      <c r="C42" s="53"/>
-      <c r="D42" s="53"/>
-      <c r="E42" s="53"/>
-      <c r="F42" s="54"/>
-      <c r="G42" s="55"/>
-      <c r="H42" s="53"/>
-    </row>
-    <row r="43" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B43" s="56" t="s">
+      <c r="C39" s="40"/>
+      <c r="D39" s="40"/>
+      <c r="E39" s="40"/>
+      <c r="F39" s="57">
+        <f>SUM(F27:F38)</f>
+        <v>31074.020778151938</v>
+      </c>
+      <c r="G39" s="41">
+        <f>G28+G31+G32+G33+G29+G30+G34</f>
+        <v>0.3107402077815194</v>
+      </c>
+      <c r="H39" s="42"/>
+    </row>
+    <row r="40" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B40" s="49"/>
+      <c r="C40" s="49"/>
+      <c r="D40" s="49"/>
+      <c r="E40" s="49"/>
+      <c r="F40" s="50"/>
+      <c r="G40" s="51"/>
+      <c r="H40" s="49"/>
+    </row>
+    <row r="41" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B41" s="52" t="s">
         <v>16</v>
       </c>
-      <c r="C43" s="57"/>
-      <c r="D43" s="57"/>
-      <c r="E43" s="57"/>
-      <c r="F43" s="58"/>
-      <c r="G43" s="59"/>
-      <c r="H43" s="60"/>
-    </row>
-    <row r="44" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="C41" s="53"/>
+      <c r="D41" s="53"/>
+      <c r="E41" s="53"/>
+      <c r="F41" s="54"/>
+      <c r="G41" s="55"/>
+      <c r="H41" s="56"/>
+    </row>
+    <row r="42" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B42" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="G42" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H42" s="12"/>
+    </row>
+    <row r="43" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B43" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="G43" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H43" s="12"/>
+    </row>
+    <row r="44" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B44" s="10" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="G44" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H44" s="12"/>
     </row>
-    <row r="45" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B45" s="10" t="s">
-        <v>2</v>
+        <v>18</v>
       </c>
       <c r="G45" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H45" s="12"/>
     </row>
-    <row r="46" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B46" s="10" t="s">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="G46" s="1" t="s">
         <v>14</v>
       </c>
       <c r="H46" s="12"/>
     </row>
-    <row r="47" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B47" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="G47" s="1" t="s">
+    <row r="47" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B47" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="C47" s="27"/>
+      <c r="D47" s="27"/>
+      <c r="E47" s="27"/>
+      <c r="F47" s="27"/>
+      <c r="G47" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="H47" s="12"/>
-    </row>
-    <row r="48" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B48" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="G48" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H48" s="12"/>
-    </row>
-    <row r="49" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B49" s="29" t="s">
-        <v>15</v>
-      </c>
-      <c r="C49" s="30"/>
-      <c r="D49" s="30"/>
-      <c r="E49" s="30"/>
-      <c r="F49" s="30"/>
-      <c r="G49" s="31" t="s">
-        <v>14</v>
-      </c>
-      <c r="H49" s="32"/>
-    </row>
-    <row r="51" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="H47" s="29"/>
+    </row>
+    <row r="49" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C49" s="1"/>
+      <c r="D49" s="4"/>
+    </row>
+    <row r="50" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C50" s="1"/>
+      <c r="D50" s="4"/>
+    </row>
+    <row r="51" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C51" s="1"/>
       <c r="D51" s="4"/>
     </row>
-    <row r="52" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C52" s="1"/>
       <c r="D52" s="4"/>
     </row>
-    <row r="53" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="C53" s="1"/>
-      <c r="D53" s="4"/>
-    </row>
-    <row r="54" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="C54" s="1"/>
-      <c r="D54" s="4"/>
-    </row>
-    <row r="59" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B59" s="86" t="s">
+    <row r="57" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B57" s="85" t="s">
         <v>7</v>
       </c>
-      <c r="C59" s="86"/>
-    </row>
-    <row r="60" spans="2:8" ht="11.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C57" s="85"/>
+    </row>
+    <row r="58" spans="2:4" ht="11.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B58" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="59" spans="2:4" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B59" t="s">
+        <v>1</v>
+      </c>
+      <c r="C59" s="5"/>
+    </row>
+    <row r="60" spans="2:4" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B60" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="61" spans="2:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="61" spans="2:4" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B61" t="s">
-        <v>1</v>
-      </c>
-      <c r="C61" s="5"/>
-    </row>
-    <row r="62" spans="2:8" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="62" spans="2:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B62" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="63" spans="2:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="63" spans="2:4" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B63" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="64" spans="2:8" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B64" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="65" spans="2:2" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B65" t="s">
         <v>5</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="B59:C59"/>
+    <mergeCell ref="B57:C57"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" scale="39" orientation="portrait" r:id="rId1"/>
@@ -2019,11 +1993,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.28515625" style="39" customWidth="1"/>
+    <col min="1" max="1" width="30.28515625" style="36" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" s="85" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="85" t="s">
+    <row r="1" spans="1:1" s="80" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="80" t="s">
         <v>52</v>
       </c>
     </row>

</xml_diff>

<commit_message>
feat - ajustado formula de soma da quantidade de meses pela descricao
</commit_message>
<xml_diff>
--- a/template.xlsx
+++ b/template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luan\Documents\Projetos\Entercap\ENTERCAP-Resumo-tributario\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25167A7F-5406-43DF-AFCC-405216720451}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{741ABF36-0338-4239-B39E-56A81B3F1199}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -188,9 +188,6 @@
     <t>% ICMS Venda</t>
   </si>
   <si>
-    <t>Resumo Tributário: Simples Nacional</t>
-  </si>
-  <si>
     <t>Empresa: NOME EMPRESA LTDA</t>
   </si>
   <si>
@@ -200,9 +197,6 @@
     <t>DESCRIÇÃO</t>
   </si>
   <si>
-    <t xml:space="preserve">Receita sem ST </t>
-  </si>
-  <si>
     <t>Receita com ST</t>
   </si>
   <si>
@@ -210,6 +204,12 @@
   </si>
   <si>
     <t>ICMS Mensal</t>
+  </si>
+  <si>
+    <t>Planejamento Tributário</t>
+  </si>
+  <si>
+    <t>Receita sem ST</t>
   </si>
 </sst>
 </file>
@@ -493,7 +493,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="86">
+  <cellXfs count="88">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
@@ -502,10 +502,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="4" fontId="3" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="3" fillId="4" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -520,14 +518,10 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="3" fillId="3" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="3" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -536,7 +530,6 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="3" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -547,7 +540,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="3" fillId="5" borderId="7" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -607,8 +599,34 @@
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="10" fontId="1" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="3" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="3" fillId="3" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="1" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="3" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="3" fillId="4" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="3" fillId="5" borderId="7" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1263,8 +1281,8 @@
   </sheetPr>
   <dimension ref="A1:S63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1276,12 +1294,12 @@
     <col min="6" max="6" width="16.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13.5703125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10.5703125" customWidth="1"/>
-    <col min="9" max="9" width="8.85546875" style="36"/>
+    <col min="9" max="9" width="8.85546875" style="31"/>
     <col min="10" max="10" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.7109375" style="46"/>
+    <col min="11" max="11" width="8.7109375" style="40"/>
     <col min="12" max="12" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="2.85546875" style="46" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="19.140625" style="46" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="2.85546875" style="40" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="19.140625" style="40" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="14.5703125" customWidth="1"/>
     <col min="16" max="16" width="14.5703125" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="7.85546875" bestFit="1" customWidth="1"/>
@@ -1296,7 +1314,7 @@
       <c r="O1" t="s">
         <v>40</v>
       </c>
-      <c r="P1" s="61">
+      <c r="P1" s="55">
         <f>C35</f>
         <v>0.12</v>
       </c>
@@ -1306,7 +1324,7 @@
       <c r="O2" t="s">
         <v>41</v>
       </c>
-      <c r="P2" s="61">
+      <c r="P2" s="55">
         <f>C36</f>
         <v>0.17</v>
       </c>
@@ -1316,7 +1334,7 @@
       <c r="O3" t="s">
         <v>4</v>
       </c>
-      <c r="P3" s="62">
+      <c r="P3" s="56">
         <f>H30</f>
         <v>1.6500000000000001E-2</v>
       </c>
@@ -1326,12 +1344,13 @@
       <c r="O4" t="s">
         <v>5</v>
       </c>
-      <c r="P4" s="62">
+      <c r="P4" s="56">
         <f>H29</f>
         <v>7.5999999999999998E-2</v>
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="G5" s="31"/>
       <c r="N5"/>
       <c r="O5" t="s">
         <v>37</v>
@@ -1342,6 +1361,7 @@
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="G6" s="31"/>
       <c r="N6"/>
       <c r="O6" t="s">
         <v>38</v>
@@ -1352,14 +1372,15 @@
       </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A7" s="38"/>
-      <c r="B7" s="35" t="s">
+      <c r="A7" s="33"/>
+      <c r="B7" s="30" t="s">
+        <v>49</v>
+      </c>
+      <c r="C7" s="72" t="s">
         <v>50</v>
       </c>
-      <c r="C7" s="78" t="s">
-        <v>51</v>
-      </c>
-      <c r="D7" s="38"/>
+      <c r="D7" s="33"/>
+      <c r="G7" s="31"/>
       <c r="H7" s="2"/>
       <c r="N7"/>
       <c r="O7" t="s">
@@ -1371,554 +1392,558 @@
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="N8" s="63"/>
-      <c r="O8" s="64" t="s">
+      <c r="G8" s="31"/>
+      <c r="N8" s="57"/>
+      <c r="O8" s="58" t="s">
         <v>35</v>
       </c>
-      <c r="P8" s="65" t="s">
+      <c r="P8" s="59" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="N9" s="66" t="s">
+      <c r="G9" s="31"/>
+      <c r="N9" s="60" t="s">
         <v>42</v>
       </c>
-      <c r="O9" s="59">
+      <c r="O9" s="53">
         <f>(P5-O13)</f>
         <v>880</v>
       </c>
-      <c r="P9" s="67"/>
+      <c r="P9" s="61"/>
     </row>
     <row r="10" spans="1:19" ht="21" x14ac:dyDescent="0.35">
-      <c r="B10" s="30" t="s">
-        <v>49</v>
+      <c r="B10" s="26" t="s">
+        <v>55</v>
       </c>
       <c r="C10" t="s">
         <v>34</v>
       </c>
-      <c r="N10" s="66" t="s">
+      <c r="G10" s="31"/>
+      <c r="N10" s="60" t="s">
         <v>43</v>
       </c>
       <c r="O10" s="1">
         <f>P6</f>
         <v>40000</v>
       </c>
-      <c r="P10" s="67"/>
+      <c r="P10" s="61"/>
     </row>
     <row r="11" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="N11" s="66" t="s">
+      <c r="G11" s="31"/>
+      <c r="N11" s="60" t="s">
         <v>44</v>
       </c>
-      <c r="P11" s="71">
+      <c r="P11" s="65">
         <f>(P7-P13)</f>
         <v>83000</v>
       </c>
-      <c r="R11" s="75" t="s">
+      <c r="R11" s="69" t="s">
         <v>4</v>
       </c>
-      <c r="S11" s="76">
+      <c r="S11" s="70">
         <f>(P12*P3)-(O12*P3)</f>
         <v>694.98</v>
       </c>
     </row>
     <row r="12" spans="1:19" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B12" s="13" t="s">
+      <c r="B12" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="C12" s="33"/>
-      <c r="D12" s="33"/>
-      <c r="E12" s="33"/>
-      <c r="F12" s="14"/>
-      <c r="G12" s="14"/>
-      <c r="H12" s="15"/>
-      <c r="N12" s="72" t="s">
+      <c r="C12" s="29"/>
+      <c r="D12" s="29"/>
+      <c r="E12" s="29"/>
+      <c r="F12" s="12"/>
+      <c r="G12" s="79"/>
+      <c r="H12" s="13"/>
+      <c r="N12" s="66" t="s">
         <v>46</v>
       </c>
-      <c r="O12" s="73">
+      <c r="O12" s="67">
         <f>SUM(O9:O11)</f>
         <v>40880</v>
       </c>
-      <c r="P12" s="74">
+      <c r="P12" s="68">
         <f>SUM(P11)</f>
         <v>83000</v>
       </c>
-      <c r="R12" s="75" t="s">
+      <c r="R12" s="69" t="s">
         <v>5</v>
       </c>
-      <c r="S12" s="76">
+      <c r="S12" s="70">
         <f>(P12*P4)-(O12*P4)</f>
         <v>3201.12</v>
       </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B13" s="16"/>
-      <c r="F13" s="17" t="s">
+      <c r="B13" s="14"/>
+      <c r="F13" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="G13" s="17" t="s">
+      <c r="G13" s="74" t="s">
         <v>11</v>
       </c>
-      <c r="H13" s="18" t="s">
+      <c r="H13" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="N13" s="68" t="s">
+      <c r="N13" s="62" t="s">
         <v>45</v>
       </c>
-      <c r="O13" s="69">
+      <c r="O13" s="63">
         <f>P5*P1</f>
         <v>120</v>
       </c>
-      <c r="P13" s="70">
+      <c r="P13" s="64">
         <f>P7*P2</f>
         <v>17000</v>
       </c>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B14" s="10" t="s">
+      <c r="B14" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="F14" s="44">
+      <c r="F14" s="38">
         <v>100000</v>
       </c>
-      <c r="G14" s="11">
+      <c r="G14" s="80">
         <f>F14/$F$14</f>
         <v>1</v>
       </c>
-      <c r="H14" s="18">
+      <c r="H14" s="16">
         <v>5</v>
       </c>
-      <c r="J14" s="37"/>
+      <c r="J14" s="32"/>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B15" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="F15" s="44">
+      <c r="B15" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="F15" s="38">
         <v>3000</v>
       </c>
-      <c r="G15" s="11">
+      <c r="G15" s="80">
         <f t="shared" ref="G15:G16" si="0">F15/$F$14</f>
         <v>0.03</v>
       </c>
-      <c r="H15" s="18">
+      <c r="H15" s="16">
         <v>1</v>
       </c>
-      <c r="J15" s="37"/>
+      <c r="J15" s="32"/>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B16" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="F16" s="44">
+      <c r="B16" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="F16" s="38">
         <v>4000</v>
       </c>
-      <c r="G16" s="11">
+      <c r="G16" s="80">
         <f t="shared" si="0"/>
         <v>0.04</v>
       </c>
-      <c r="H16" s="18">
+      <c r="H16" s="16">
         <v>2</v>
       </c>
-      <c r="J16" s="37"/>
+      <c r="J16" s="32"/>
     </row>
     <row r="17" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B17" s="10" t="s">
+      <c r="B17" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="F17" s="44">
+      <c r="F17" s="38">
         <v>1000</v>
       </c>
-      <c r="G17" s="11">
+      <c r="G17" s="80">
         <f>F17/$F$14</f>
         <v>0.01</v>
       </c>
-      <c r="H17" s="18">
+      <c r="H17" s="16">
         <v>5</v>
       </c>
-      <c r="J17" s="37"/>
+      <c r="J17" s="32"/>
     </row>
     <row r="18" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B18" s="10" t="s">
+      <c r="B18" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="F18" s="44">
+      <c r="F18" s="38">
         <v>2000</v>
       </c>
-      <c r="G18" s="11">
+      <c r="G18" s="80">
         <f>F18/$F$14</f>
         <v>0.02</v>
       </c>
-      <c r="H18" s="18">
+      <c r="H18" s="16">
         <v>14</v>
       </c>
     </row>
     <row r="19" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B19" s="19" t="s">
+      <c r="B19" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="C19" s="32"/>
-      <c r="D19" s="32"/>
-      <c r="E19" s="32"/>
-      <c r="F19" s="47"/>
-      <c r="G19" s="20">
+      <c r="C19" s="28"/>
+      <c r="D19" s="28"/>
+      <c r="E19" s="28"/>
+      <c r="F19" s="41"/>
+      <c r="G19" s="81">
         <f>SUM(G20:G20)</f>
         <v>0</v>
       </c>
-      <c r="H19" s="21"/>
-      <c r="K19" s="58"/>
-      <c r="L19" s="44"/>
-      <c r="M19" s="58"/>
-      <c r="N19" s="58">
+      <c r="H19" s="18"/>
+      <c r="K19" s="52"/>
+      <c r="L19" s="38"/>
+      <c r="M19" s="52"/>
+      <c r="N19" s="52">
         <f>+K19*L19</f>
         <v>0</v>
       </c>
     </row>
     <row r="20" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B20" s="81" t="s">
-        <v>56</v>
-      </c>
-      <c r="F20" s="82"/>
-      <c r="G20" s="83"/>
-      <c r="H20" s="84"/>
+      <c r="B20" s="75" t="s">
+        <v>54</v>
+      </c>
+      <c r="F20" s="76"/>
+      <c r="G20" s="82"/>
+      <c r="H20" s="77"/>
     </row>
     <row r="21" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B21" s="19" t="s">
+      <c r="B21" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="C21" s="32"/>
-      <c r="D21" s="32"/>
-      <c r="E21" s="32"/>
-      <c r="F21" s="47"/>
-      <c r="G21" s="20"/>
-      <c r="H21" s="21"/>
+      <c r="C21" s="28"/>
+      <c r="D21" s="28"/>
+      <c r="E21" s="28"/>
+      <c r="F21" s="41"/>
+      <c r="G21" s="81"/>
+      <c r="H21" s="18"/>
     </row>
     <row r="22" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B22" s="10" t="s">
+      <c r="B22" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="C22" s="45">
+      <c r="C22" s="39">
         <f>F22/16</f>
         <v>2500</v>
       </c>
-      <c r="D22" s="46" t="s">
+      <c r="D22" s="40" t="s">
         <v>26</v>
       </c>
-      <c r="F22" s="44">
+      <c r="F22" s="38">
         <f>H22*F14</f>
         <v>40000</v>
       </c>
-      <c r="G22" s="11">
+      <c r="G22" s="80">
         <f>F22/F14</f>
         <v>0.4</v>
       </c>
-      <c r="H22" s="60">
+      <c r="H22" s="54">
         <v>0.4</v>
       </c>
     </row>
     <row r="23" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B23" s="10" t="s">
+      <c r="B23" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="C23" s="45">
+      <c r="C23" s="39">
         <f>F23/16</f>
         <v>3562.4999999999995</v>
       </c>
-      <c r="D23" s="46" t="s">
+      <c r="D23" s="40" t="s">
         <v>26</v>
       </c>
-      <c r="F23" s="44">
+      <c r="F23" s="38">
         <f>G23*F14</f>
         <v>56999.999999999993</v>
       </c>
-      <c r="G23" s="11">
+      <c r="G23" s="80">
         <f>(100%-SUM(G17:G18,G19,G22))</f>
         <v>0.56999999999999995</v>
       </c>
-      <c r="H23" s="12"/>
+      <c r="H23" s="10"/>
     </row>
     <row r="24" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="22" t="s">
+      <c r="B24" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="C24" s="23"/>
-      <c r="D24" s="23"/>
-      <c r="E24" s="23"/>
-      <c r="F24" s="48"/>
-      <c r="G24" s="34">
+      <c r="C24" s="20"/>
+      <c r="D24" s="20"/>
+      <c r="E24" s="20"/>
+      <c r="F24" s="42"/>
+      <c r="G24" s="83">
         <f>100% - SUM(G20:G20,G22:G23)</f>
         <v>3.0000000000000027E-2</v>
       </c>
-      <c r="H24" s="24"/>
+      <c r="H24" s="21"/>
     </row>
     <row r="25" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F25" s="1"/>
-      <c r="G25" s="4"/>
+      <c r="G25" s="84"/>
     </row>
     <row r="26" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B26" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C26" s="31"/>
-      <c r="D26" s="31"/>
-      <c r="E26" s="31"/>
+      <c r="C26" s="27"/>
+      <c r="D26" s="27"/>
+      <c r="E26" s="27"/>
       <c r="F26" s="7"/>
-      <c r="G26" s="8"/>
-      <c r="H26" s="9"/>
+      <c r="G26" s="85"/>
+      <c r="H26" s="8"/>
     </row>
     <row r="27" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B27" s="10"/>
+      <c r="B27" s="9"/>
       <c r="F27" s="1"/>
-      <c r="G27" s="25" t="s">
+      <c r="G27" s="78" t="s">
         <v>11</v>
       </c>
-      <c r="H27" s="12"/>
+      <c r="H27" s="10"/>
     </row>
     <row r="28" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B28" s="10" t="s">
+      <c r="B28" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="F28" s="44">
+      <c r="F28" s="38">
         <f>$F$14*H28</f>
         <v>1617.9207781519399</v>
       </c>
-      <c r="G28" s="11">
+      <c r="G28" s="80">
         <f>F28/F14</f>
         <v>1.6179207781519399E-2</v>
       </c>
-      <c r="H28" s="79">
+      <c r="H28" s="73">
         <v>1.6179207781519399E-2</v>
       </c>
-      <c r="L28" s="43"/>
-      <c r="O28" s="77"/>
-      <c r="P28" s="77"/>
+      <c r="L28" s="37"/>
+      <c r="O28" s="71"/>
+      <c r="P28" s="71"/>
     </row>
     <row r="29" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B29" s="10" t="s">
+      <c r="B29" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="F29" s="44">
+      <c r="F29" s="38">
         <f>S12</f>
         <v>3201.12</v>
       </c>
-      <c r="G29" s="11">
+      <c r="G29" s="80">
         <f>F29/$F$14</f>
         <v>3.2011199999999997E-2</v>
       </c>
-      <c r="H29" s="79">
+      <c r="H29" s="73">
         <v>7.5999999999999998E-2</v>
       </c>
       <c r="L29" s="3"/>
-      <c r="O29" s="77"/>
-      <c r="P29" s="77"/>
+      <c r="O29" s="71"/>
+      <c r="P29" s="71"/>
     </row>
     <row r="30" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B30" s="10" t="s">
+      <c r="B30" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="F30" s="44">
+      <c r="F30" s="38">
         <f>S11</f>
         <v>694.98</v>
       </c>
-      <c r="G30" s="11">
+      <c r="G30" s="80">
         <f t="shared" ref="G30:G32" si="1">F30/$F$14</f>
         <v>6.9497999999999999E-3</v>
       </c>
-      <c r="H30" s="79">
+      <c r="H30" s="73">
         <v>1.6500000000000001E-2</v>
       </c>
-      <c r="O30" s="77"/>
-      <c r="P30" s="77"/>
+      <c r="O30" s="71"/>
+      <c r="P30" s="71"/>
     </row>
     <row r="31" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B31" s="10" t="s">
+      <c r="B31" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="F31" s="44">
+      <c r="F31" s="38">
         <f>IF(F23&gt;0,F23*H31,0)</f>
         <v>8549.9999999999982</v>
       </c>
-      <c r="G31" s="11">
+      <c r="G31" s="80">
         <f t="shared" si="1"/>
         <v>8.5499999999999979E-2</v>
       </c>
-      <c r="H31" s="79">
+      <c r="H31" s="73">
         <v>0.15</v>
       </c>
-      <c r="O31" s="77"/>
-      <c r="P31" s="77"/>
+      <c r="O31" s="71"/>
+      <c r="P31" s="71"/>
     </row>
     <row r="32" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B32" s="10" t="s">
+      <c r="B32" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="F32" s="44">
+      <c r="F32" s="38">
         <f>IF(F23&gt;0,F23*H32,0)</f>
         <v>5129.9999999999991</v>
       </c>
-      <c r="G32" s="11">
+      <c r="G32" s="80">
         <f t="shared" si="1"/>
         <v>5.1299999999999991E-2</v>
       </c>
-      <c r="H32" s="79">
+      <c r="H32" s="73">
         <v>0.09</v>
       </c>
-      <c r="O32" s="77"/>
-      <c r="P32" s="77"/>
+      <c r="O32" s="71"/>
+      <c r="P32" s="71"/>
     </row>
     <row r="33" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B33" s="10" t="s">
+      <c r="B33" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="F33" s="44">
+      <c r="F33" s="38">
         <f>+(H33*F14)-(F17*12%)</f>
         <v>11880</v>
       </c>
-      <c r="G33" s="11">
+      <c r="G33" s="80">
         <f>F33/$F$14</f>
         <v>0.1188</v>
       </c>
-      <c r="H33" s="79">
+      <c r="H33" s="73">
         <v>0.12</v>
       </c>
       <c r="J33" s="4"/>
     </row>
     <row r="34" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B34" s="10"/>
+      <c r="B34" s="9"/>
       <c r="F34" s="1"/>
-      <c r="G34" s="11"/>
-      <c r="H34" s="12"/>
+      <c r="G34" s="80"/>
+      <c r="H34" s="10"/>
       <c r="J34" s="4" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="35" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B35" s="10" t="s">
+      <c r="B35" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="C35" s="61">
+      <c r="C35" s="55">
         <v>0.12</v>
       </c>
       <c r="F35" s="1"/>
-      <c r="G35" s="11"/>
-      <c r="H35" s="12"/>
+      <c r="G35" s="80"/>
+      <c r="H35" s="10"/>
     </row>
     <row r="36" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B36" s="10" t="s">
+      <c r="B36" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="C36" s="61">
+      <c r="C36" s="55">
         <v>0.17</v>
       </c>
       <c r="F36" s="1"/>
-      <c r="G36" s="11"/>
-      <c r="H36" s="12"/>
+      <c r="G36" s="80"/>
+      <c r="H36" s="10"/>
     </row>
     <row r="37" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B37" s="10"/>
+      <c r="B37" s="9"/>
       <c r="F37" s="1"/>
-      <c r="G37" s="11"/>
-      <c r="H37" s="12"/>
+      <c r="G37" s="80"/>
+      <c r="H37" s="10"/>
     </row>
     <row r="38" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B38" s="10"/>
+      <c r="B38" s="9"/>
       <c r="F38" s="1"/>
-      <c r="G38" s="11"/>
-      <c r="H38" s="12"/>
+      <c r="G38" s="80"/>
+      <c r="H38" s="10"/>
     </row>
     <row r="39" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B39" s="39" t="s">
+      <c r="B39" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="C39" s="40"/>
-      <c r="D39" s="40"/>
-      <c r="E39" s="40"/>
-      <c r="F39" s="57">
+      <c r="C39" s="35"/>
+      <c r="D39" s="35"/>
+      <c r="E39" s="35"/>
+      <c r="F39" s="51">
         <f>SUM(F27:F38)</f>
         <v>31074.020778151938</v>
       </c>
-      <c r="G39" s="41">
+      <c r="G39" s="86">
         <f>G28+G31+G32+G33+G29+G30+G34</f>
         <v>0.3107402077815194</v>
       </c>
-      <c r="H39" s="42"/>
+      <c r="H39" s="36"/>
     </row>
     <row r="40" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B40" s="49"/>
-      <c r="C40" s="49"/>
-      <c r="D40" s="49"/>
-      <c r="E40" s="49"/>
-      <c r="F40" s="50"/>
-      <c r="G40" s="51"/>
-      <c r="H40" s="49"/>
+      <c r="B40" s="43"/>
+      <c r="C40" s="43"/>
+      <c r="D40" s="43"/>
+      <c r="E40" s="43"/>
+      <c r="F40" s="44"/>
+      <c r="G40" s="45"/>
+      <c r="H40" s="43"/>
     </row>
     <row r="41" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B41" s="52" t="s">
+      <c r="B41" s="46" t="s">
         <v>16</v>
       </c>
-      <c r="C41" s="53"/>
-      <c r="D41" s="53"/>
-      <c r="E41" s="53"/>
-      <c r="F41" s="54"/>
-      <c r="G41" s="55"/>
-      <c r="H41" s="56"/>
+      <c r="C41" s="47"/>
+      <c r="D41" s="47"/>
+      <c r="E41" s="47"/>
+      <c r="F41" s="48"/>
+      <c r="G41" s="49"/>
+      <c r="H41" s="50"/>
     </row>
     <row r="42" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B42" s="10" t="s">
+      <c r="B42" s="9" t="s">
         <v>12</v>
       </c>
       <c r="G42" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="H42" s="12"/>
+      <c r="H42" s="10"/>
     </row>
     <row r="43" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B43" s="10" t="s">
+      <c r="B43" s="9" t="s">
         <v>2</v>
       </c>
       <c r="G43" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="H43" s="12"/>
+      <c r="H43" s="10"/>
     </row>
     <row r="44" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B44" s="10" t="s">
+      <c r="B44" s="9" t="s">
         <v>17</v>
       </c>
       <c r="G44" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H44" s="12"/>
+      <c r="H44" s="10"/>
     </row>
     <row r="45" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B45" s="10" t="s">
+      <c r="B45" s="9" t="s">
         <v>18</v>
       </c>
       <c r="G45" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H45" s="12"/>
+      <c r="H45" s="10"/>
     </row>
     <row r="46" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B46" s="10" t="s">
+      <c r="B46" s="9" t="s">
         <v>4</v>
       </c>
       <c r="G46" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H46" s="12"/>
+      <c r="H46" s="10"/>
     </row>
     <row r="47" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B47" s="26" t="s">
+      <c r="B47" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="C47" s="27"/>
-      <c r="D47" s="27"/>
-      <c r="E47" s="27"/>
-      <c r="F47" s="27"/>
-      <c r="G47" s="28" t="s">
+      <c r="C47" s="23"/>
+      <c r="D47" s="23"/>
+      <c r="E47" s="23"/>
+      <c r="F47" s="23"/>
+      <c r="G47" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="H47" s="29"/>
+      <c r="H47" s="25"/>
     </row>
     <row r="49" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C49" s="1"/>
@@ -1937,10 +1962,10 @@
       <c r="D52" s="4"/>
     </row>
     <row r="57" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B57" s="85" t="s">
+      <c r="B57" s="87" t="s">
         <v>7</v>
       </c>
-      <c r="C57" s="85"/>
+      <c r="C57" s="87"/>
     </row>
     <row r="58" spans="2:4" ht="11.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B58" t="s">
@@ -1993,12 +2018,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.28515625" style="36" customWidth="1"/>
+    <col min="1" max="1" width="30.28515625" style="31" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="80" t="s">
-        <v>52</v>
+    <row r="1" spans="1:1" s="74" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="74" t="s">
+        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat - agora a funcao de salvar ajusta o width da aba dados - agora o custo fixo é calculado
</commit_message>
<xml_diff>
--- a/template.xlsx
+++ b/template.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luan\Documents\Projetos\Entercap\ENTERCAP-Resumo-tributario\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{741ABF36-0338-4239-B39E-56A81B3F1199}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{996B96A5-D4F6-4DC3-8F89-A1DC91F3297B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Apresentação" sheetId="4" r:id="rId1"/>
     <sheet name="Dados" sheetId="7" r:id="rId2"/>
+    <sheet name="Tributos sobre vendas" sheetId="8" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="CNPJ">Apresentação!$C$7</definedName>
@@ -38,8 +39,30 @@
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="57">
   <si>
     <t>COMPRAS</t>
   </si>
@@ -1282,7 +1305,7 @@
   <dimension ref="A1:S63"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1368,7 +1391,7 @@
       </c>
       <c r="P6" s="1">
         <f>F22</f>
-        <v>40000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
@@ -1425,7 +1448,7 @@
       </c>
       <c r="O10" s="1">
         <f>P6</f>
-        <v>40000</v>
+        <v>0</v>
       </c>
       <c r="P10" s="61"/>
     </row>
@@ -1443,7 +1466,7 @@
       </c>
       <c r="S11" s="70">
         <f>(P12*P3)-(O12*P3)</f>
-        <v>694.98</v>
+        <v>1354.98</v>
       </c>
     </row>
     <row r="12" spans="1:19" ht="18.75" x14ac:dyDescent="0.3">
@@ -1461,7 +1484,7 @@
       </c>
       <c r="O12" s="67">
         <f>SUM(O9:O11)</f>
-        <v>40880</v>
+        <v>880</v>
       </c>
       <c r="P12" s="68">
         <f>SUM(P11)</f>
@@ -1472,7 +1495,7 @@
       </c>
       <c r="S12" s="70">
         <f>(P12*P4)-(O12*P4)</f>
-        <v>3201.12</v>
+        <v>6241.12</v>
       </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
@@ -1585,9 +1608,9 @@
       <c r="D19" s="28"/>
       <c r="E19" s="28"/>
       <c r="F19" s="41"/>
-      <c r="G19" s="81">
-        <f>SUM(G20:G20)</f>
-        <v>0</v>
+      <c r="G19" s="81" cm="1">
+        <f t="array" ref="G19">SUMPRODUCT(SUMIF( B13:B18, 'Tributos sobre vendas'!A1:A40, G13:G18))</f>
+        <v>0.06</v>
       </c>
       <c r="H19" s="18"/>
       <c r="K19" s="52"/>
@@ -1623,21 +1646,21 @@
       </c>
       <c r="C22" s="39">
         <f>F22/16</f>
-        <v>2500</v>
+        <v>0</v>
       </c>
       <c r="D22" s="40" t="s">
         <v>26</v>
       </c>
       <c r="F22" s="38">
-        <f>H22*F14</f>
-        <v>40000</v>
+        <f>VLOOKUP("FATURAMENTO*",B13:F50,5) * H22</f>
+        <v>0</v>
       </c>
       <c r="G22" s="80">
         <f>F22/F14</f>
-        <v>0.4</v>
+        <v>0</v>
       </c>
       <c r="H22" s="54">
-        <v>0.4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="2:16" x14ac:dyDescent="0.25">
@@ -1646,18 +1669,18 @@
       </c>
       <c r="C23" s="39">
         <f>F23/16</f>
-        <v>3562.4999999999995</v>
+        <v>5687.5</v>
       </c>
       <c r="D23" s="40" t="s">
         <v>26</v>
       </c>
       <c r="F23" s="38">
         <f>G23*F14</f>
-        <v>56999.999999999993</v>
+        <v>91000</v>
       </c>
       <c r="G23" s="80">
         <f>(100%-SUM(G17:G18,G19,G22))</f>
-        <v>0.56999999999999995</v>
+        <v>0.91</v>
       </c>
       <c r="H23" s="10"/>
     </row>
@@ -1671,7 +1694,7 @@
       <c r="F24" s="42"/>
       <c r="G24" s="83">
         <f>100% - SUM(G20:G20,G22:G23)</f>
-        <v>3.0000000000000027E-2</v>
+        <v>8.9999999999999969E-2</v>
       </c>
       <c r="H24" s="21"/>
     </row>
@@ -1723,11 +1746,11 @@
       </c>
       <c r="F29" s="38">
         <f>S12</f>
-        <v>3201.12</v>
+        <v>6241.12</v>
       </c>
       <c r="G29" s="80">
         <f>F29/$F$14</f>
-        <v>3.2011199999999997E-2</v>
+        <v>6.24112E-2</v>
       </c>
       <c r="H29" s="73">
         <v>7.5999999999999998E-2</v>
@@ -1742,11 +1765,11 @@
       </c>
       <c r="F30" s="38">
         <f>S11</f>
-        <v>694.98</v>
+        <v>1354.98</v>
       </c>
       <c r="G30" s="80">
         <f t="shared" ref="G30:G32" si="1">F30/$F$14</f>
-        <v>6.9497999999999999E-3</v>
+        <v>1.3549800000000001E-2</v>
       </c>
       <c r="H30" s="73">
         <v>1.6500000000000001E-2</v>
@@ -1760,11 +1783,11 @@
       </c>
       <c r="F31" s="38">
         <f>IF(F23&gt;0,F23*H31,0)</f>
-        <v>8549.9999999999982</v>
+        <v>13650</v>
       </c>
       <c r="G31" s="80">
         <f t="shared" si="1"/>
-        <v>8.5499999999999979E-2</v>
+        <v>0.13650000000000001</v>
       </c>
       <c r="H31" s="73">
         <v>0.15</v>
@@ -1778,11 +1801,11 @@
       </c>
       <c r="F32" s="38">
         <f>IF(F23&gt;0,F23*H32,0)</f>
-        <v>5129.9999999999991</v>
+        <v>8190</v>
       </c>
       <c r="G32" s="80">
         <f t="shared" si="1"/>
-        <v>5.1299999999999991E-2</v>
+        <v>8.1900000000000001E-2</v>
       </c>
       <c r="H32" s="73">
         <v>0.09</v>
@@ -1859,11 +1882,11 @@
       <c r="E39" s="35"/>
       <c r="F39" s="51">
         <f>SUM(F27:F38)</f>
-        <v>31074.020778151938</v>
+        <v>42934.020778151942</v>
       </c>
       <c r="G39" s="86">
         <f>G28+G31+G32+G33+G29+G30+G34</f>
-        <v>0.3107402077815194</v>
+        <v>0.42934020778151943</v>
       </c>
       <c r="H39" s="36"/>
     </row>
@@ -2030,4 +2053,32 @@
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFE287BE-10DF-43CE-BB1E-86F8F9F60678}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A21" sqref="A21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="30.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
- atualizar_inss - atualizar_irpj
</commit_message>
<xml_diff>
--- a/template.xlsx
+++ b/template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luan\Documents\Projetos\Entercap\ENTERCAP-Resumo-tributario\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91B72629-56FE-4BEF-9DAA-EEFBE97F19FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27292D69-4221-4B48-A265-D3C3019B6BFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1308,7 +1308,7 @@
   <dimension ref="A1:S63"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+      <selection activeCell="I34" sqref="I34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
atualizar_icms_compra()         atualizar_icms_venda()         atualizar_pis()         atualizar_cofins()         atualizar_compras()         atualizar_despesas()
</commit_message>
<xml_diff>
--- a/template.xlsx
+++ b/template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luan\Documents\Projetos\Entercap\ENTERCAP-Resumo-tributario\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3921671E-1866-43DA-A1B3-25534B947FD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8CA5190-4265-4361-9464-40489C921620}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1305,7 +1305,7 @@
   <dimension ref="A1:S63"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="J34" sqref="J34"/>
+      <selection activeCell="N19" sqref="N19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1326,7 +1326,7 @@
     <col min="15" max="15" width="14.5703125" customWidth="1"/>
     <col min="16" max="16" width="14.5703125" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="15" customWidth="1"/>
     <col min="16377" max="16377" width="17.5703125" bestFit="1" customWidth="1"/>
     <col min="16378" max="16379" width="16.140625" bestFit="1" customWidth="1"/>
     <col min="16382" max="16382" width="10.5703125" bestFit="1" customWidth="1"/>

</xml_diff>

<commit_message>
feat - ajustado calculo lucro teorico
</commit_message>
<xml_diff>
--- a/template.xlsx
+++ b/template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luan\Documents\Projetos\Entercap\ENTERCAP-Resumo-tributario\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8CA5190-4265-4361-9464-40489C921620}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{604555DA-DC52-4949-BF3F-3657717D94FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="57">
   <si>
     <t>COMPRAS</t>
   </si>
@@ -232,7 +232,7 @@
     <t>Receita sem ST</t>
   </si>
   <si>
-    <t>0211 - IRPF - Carnê-Leão</t>
+    <t>Simples Nacional</t>
   </si>
 </sst>
 </file>
@@ -516,7 +516,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="88">
+  <cellXfs count="89">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
@@ -652,6 +652,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -991,8 +994,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>13155</xdr:colOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>477499</xdr:colOff>
       <xdr:row>5</xdr:row>
       <xdr:rowOff>59690</xdr:rowOff>
     </xdr:to>
@@ -1305,7 +1308,7 @@
   <dimension ref="A1:S63"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="N19" sqref="N19"/>
+      <selection activeCell="O26" sqref="O26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1314,7 +1317,7 @@
     <col min="3" max="3" width="16" customWidth="1"/>
     <col min="4" max="4" width="8.5703125" customWidth="1"/>
     <col min="5" max="5" width="11.42578125" customWidth="1"/>
-    <col min="6" max="6" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.140625" customWidth="1"/>
     <col min="7" max="7" width="13.5703125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10.5703125" customWidth="1"/>
     <col min="9" max="9" width="8.85546875" style="31"/>
@@ -1324,9 +1327,10 @@
     <col min="13" max="13" width="2.85546875" style="40" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="19.140625" style="40" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="14.5703125" customWidth="1"/>
-    <col min="16" max="16" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="19.42578125" customWidth="1"/>
+    <col min="17" max="17" width="13.42578125" customWidth="1"/>
     <col min="18" max="18" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="15" customWidth="1"/>
+    <col min="19" max="19" width="21.5703125" customWidth="1"/>
     <col min="16377" max="16377" width="17.5703125" bestFit="1" customWidth="1"/>
     <col min="16378" max="16379" width="16.140625" bestFit="1" customWidth="1"/>
     <col min="16382" max="16382" width="10.5703125" bestFit="1" customWidth="1"/>
@@ -1461,6 +1465,10 @@
         <f>(P7-P13)</f>
         <v>83000</v>
       </c>
+      <c r="Q11" s="88">
+        <f>P11/F14</f>
+        <v>0.83</v>
+      </c>
       <c r="R11" s="69" t="s">
         <v>4</v>
       </c>
@@ -1610,7 +1618,7 @@
       <c r="F19" s="41"/>
       <c r="G19" s="81" cm="1">
         <f t="array" ref="G19">SUMPRODUCT(SUMIF( B13:B18, 'Tributos sobre vendas'!A1:A40, G13:G18))</f>
-        <v>0.03</v>
+        <v>0</v>
       </c>
       <c r="H19" s="18"/>
       <c r="K19" s="52"/>
@@ -1693,7 +1701,7 @@
       <c r="F24" s="42"/>
       <c r="G24" s="83">
         <f>SUM(G19,G20)</f>
-        <v>0.03</v>
+        <v>0</v>
       </c>
       <c r="H24" s="21"/>
     </row>
@@ -2054,10 +2062,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFE287BE-10DF-43CE-BB1E-86F8F9F60678}">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2070,11 +2078,6 @@
         <v>56</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>55</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>